<commit_message>
min daily dose update
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase_result.xlsx
+++ b/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase_result.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="257">
   <si>
     <t>Testcase_id</t>
   </si>
@@ -856,40 +856,34 @@
     <t>Tenant ID:</t>
   </si>
   <si>
-    <t>S4 active1</t>
-  </si>
-  <si>
-    <t>S4</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Liquid</t>
-  </si>
-  <si>
-    <t>Inhalant</t>
+    <t>S1 active1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>S1 active2</t>
+  </si>
+  <si>
+    <t>S2 active1</t>
+  </si>
+  <si>
+    <t>S1</t>
   </si>
   <si>
     <t>E5</t>
   </si>
   <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>S4 active2</t>
-  </si>
-  <si>
-    <t>Liquid active1</t>
-  </si>
-  <si>
-    <t>Liquid active3</t>
-  </si>
-  <si>
-    <t>Inhalant active1</t>
-  </si>
-  <si>
-    <t>Inhalant active4</t>
+    <t>S2 active2</t>
   </si>
 </sst>
 </file>
@@ -899,7 +893,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="182" x14ac:knownFonts="1">
+  <fonts count="180" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1713,117 +1707,7 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
+      <color indexed="10"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1853,7 +1737,107 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="17"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -2077,7 +2061,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="435">
+  <cellXfs count="433">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -2860,8 +2844,6 @@
     <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="181" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -10924,67 +10906,69 @@
         <v>0.005714286584407091</v>
       </c>
       <c r="G42" s="252" t="n">
-        <v>1.1111020026569237E-4</v>
+        <v>1.6000130122925156E-4</v>
       </c>
       <c r="H42" s="253" t="n">
-        <v>199.99836047824627</v>
+        <v>80.00065061462577</v>
       </c>
       <c r="I42" s="253" t="n">
-        <v>2.8168783165950177E-4</v>
-      </c>
-      <c r="J42" s="253" t="s">
-        <v>249</v>
-      </c>
-      <c r="K42" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="L42" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="M42" s="253" t="s">
-        <v>249</v>
-      </c>
-      <c r="N42" s="298"/>
+        <v>1.1851948239203817E-4</v>
+      </c>
+      <c r="J42" s="253" t="n">
+        <v>0.005714286584407091</v>
+      </c>
+      <c r="K42" s="252" t="n">
+        <v>1.6000002506189048E-4</v>
+      </c>
+      <c r="L42" s="252" t="n">
+        <v>80.00000762939453</v>
+      </c>
+      <c r="M42" s="253" t="n">
+        <v>7.646356825716794E-4</v>
+      </c>
+      <c r="N42" s="401" t="s">
+        <v>59</v>
+      </c>
       <c r="O42" s="64"/>
       <c r="P42" s="232"/>
       <c r="Q42" s="243" t="s">
         <v>247</v>
       </c>
       <c r="R42" s="381" t="s">
-        <v>252</v>
+        <v>225</v>
       </c>
       <c r="S42" s="381" t="n">
-        <v>35000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="T42" s="381" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="U42" s="381" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V42" s="381" t="n">
         <v>60.0</v>
       </c>
-      <c r="U42" s="381" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="V42" s="381" t="n">
-        <v>70.0</v>
-      </c>
       <c r="W42" s="381" t="n">
-        <v>0.0013136290945112705</v>
+        <v>0.00592597434297204</v>
       </c>
       <c r="X42" s="381" t="n">
-        <v>4.378763648370902E-5</v>
+        <v>2.96298717148602E-4</v>
       </c>
       <c r="Y42" s="382" t="n">
-        <v>1.0946909242193215E-5</v>
+        <v>1.9753248125198297E-5</v>
       </c>
       <c r="Z42" s="381" t="n">
-        <v>0.0013136290945112705</v>
+        <v>0.03823178634047508</v>
       </c>
       <c r="AA42" s="381" t="n">
-        <v>4.378763696877286E-5</v>
+        <v>0.0019115892937406898</v>
       </c>
       <c r="AB42" s="383" t="n">
-        <v>1.0946909242193215E-5</v>
+        <v>1.2743928527925164E-4</v>
       </c>
       <c r="AC42" s="402" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD42" s="64"/>
       <c r="AE42" s="50"/>
@@ -11006,75 +10990,79 @@
       <c r="B43" s="276" t="s">
         <v>245</v>
       </c>
-      <c r="D43" s="34"/>
+      <c r="D43" s="34" t="s">
+        <v>252</v>
+      </c>
       <c r="E43" s="34" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F43" s="253" t="n">
-        <v>0.005714286584407091</v>
+        <v>0.011428573168814182</v>
       </c>
       <c r="G43" s="252" t="n">
-        <v>1.5873018290019698E-5</v>
+        <v>3.200026024585031E-4</v>
       </c>
       <c r="H43" s="253" t="n">
-        <v>15.873018290019699</v>
+        <v>160.00130122925154</v>
       </c>
       <c r="I43" s="254" t="n">
-        <v>3.648969721843609E-5</v>
-      </c>
-      <c r="J43" s="253" t="s">
-        <v>249</v>
-      </c>
-      <c r="K43" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="L43" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="M43" s="254" t="s">
-        <v>249</v>
-      </c>
-      <c r="N43" s="272"/>
+        <v>2.3703896478407635E-4</v>
+      </c>
+      <c r="J43" s="253" t="n">
+        <v>0.011428573168814182</v>
+      </c>
+      <c r="K43" s="252" t="n">
+        <v>3.2000005012378097E-4</v>
+      </c>
+      <c r="L43" s="252" t="n">
+        <v>160.00001525878906</v>
+      </c>
+      <c r="M43" s="254" t="n">
+        <v>0.0015292713651433587</v>
+      </c>
+      <c r="N43" s="409" t="s">
+        <v>59</v>
+      </c>
       <c r="O43" s="64"/>
       <c r="P43" s="232"/>
       <c r="Q43" s="243" t="s">
         <v>247</v>
       </c>
       <c r="R43" s="381" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="S43" s="381" t="n">
-        <v>75000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="T43" s="381" t="n">
         <v>60.0</v>
       </c>
       <c r="U43" s="381" t="n">
-        <v>100.0</v>
+        <v>40.0</v>
       </c>
       <c r="V43" s="381" t="n">
-        <v>30.0</v>
+        <v>20.0</v>
       </c>
       <c r="W43" s="381" t="n">
-        <v>0.0013136290945112705</v>
+        <v>0.007111168932169676</v>
       </c>
       <c r="X43" s="381" t="n">
-        <v>1.3136290945112706E-5</v>
+        <v>1.7777922330424188E-4</v>
       </c>
       <c r="Y43" s="382" t="n">
-        <v>5.4734548029955477E-5</v>
+        <v>1.481493527535349E-4</v>
       </c>
       <c r="Z43" s="381" t="n">
-        <v>0.0013136290945112705</v>
+        <v>0.04587814211845398</v>
       </c>
       <c r="AA43" s="381" t="n">
-        <v>1.3136291272530798E-5</v>
+        <v>0.0011469535529613495</v>
       </c>
       <c r="AB43" s="383" t="n">
-        <v>5.473454439197667E-5</v>
+        <v>9.557946468703449E-4</v>
       </c>
       <c r="AC43" s="403" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD43" s="64"/>
       <c r="AE43" s="50"/>
@@ -11094,36 +11082,38 @@
         <v>3</v>
       </c>
       <c r="B44" s="276"/>
-      <c r="D44" s="34"/>
+      <c r="D44" s="34" t="s">
+        <v>253</v>
+      </c>
       <c r="E44" s="34" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F44" s="252" t="n">
-        <v>0.005714286584407091</v>
+        <v>0.007142857648432255</v>
       </c>
       <c r="G44" s="252" t="n">
-        <v>7.936509145009849E-6</v>
+        <v>1.3888773901405367E-4</v>
       </c>
       <c r="H44" s="253" t="n">
-        <v>9.52381097401182</v>
+        <v>249.9979302252966</v>
       </c>
       <c r="I44" s="253" t="n">
-        <v>2.1893818331061655E-5</v>
+        <v>3.703673040374765E-4</v>
       </c>
       <c r="J44" s="253" t="n">
-        <v>0.005714286584407091</v>
+        <v>0.007142857648432255</v>
       </c>
       <c r="K44" s="252" t="n">
-        <v>7.936509064165875E-6</v>
+        <v>1.3888889225199819E-4</v>
       </c>
       <c r="L44" s="252" t="n">
-        <v>9.523811340332031</v>
+        <v>250.0</v>
       </c>
       <c r="M44" s="253" t="n">
-        <v>2.189381848438643E-5</v>
-      </c>
-      <c r="N44" s="401" t="s">
-        <v>56</v>
+        <v>0.002389486413449049</v>
+      </c>
+      <c r="N44" s="417" t="s">
+        <v>59</v>
       </c>
       <c r="O44" s="64"/>
       <c r="P44" s="232"/>
@@ -11131,40 +11121,40 @@
         <v>247</v>
       </c>
       <c r="R44" s="381" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="S44" s="381" t="n">
-        <v>100000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="T44" s="381" t="n">
-        <v>20.0</v>
+        <v>60.0</v>
       </c>
       <c r="U44" s="381" t="n">
-        <v>50.0</v>
+        <v>100.0</v>
       </c>
       <c r="V44" s="381" t="n">
         <v>30.0</v>
       </c>
       <c r="W44" s="381" t="n">
-        <v>4.378763842396438E-4</v>
+        <v>0.007111168932169676</v>
       </c>
       <c r="X44" s="381" t="n">
-        <v>8.757527684792876E-6</v>
+        <v>7.111168932169676E-5</v>
       </c>
       <c r="Y44" s="382" t="n">
-        <v>7.297939737327397E-5</v>
+        <v>2.962987346109003E-4</v>
       </c>
       <c r="Z44" s="381" t="n">
-        <v>4.3787635513581336E-4</v>
+        <v>0.04587814211845398</v>
       </c>
       <c r="AA44" s="381" t="n">
-        <v>8.757527211855631E-6</v>
+        <v>4.587814037222415E-4</v>
       </c>
       <c r="AB44" s="383" t="n">
-        <v>7.297939737327397E-5</v>
+        <v>0.0019115892937406898</v>
       </c>
       <c r="AC44" s="404" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD44" s="64"/>
       <c r="AE44" s="50"/>
@@ -11185,76 +11175,78 @@
       </c>
       <c r="B45" s="276"/>
       <c r="D45" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="E45" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="E45" s="34" t="s">
-        <v>248</v>
-      </c>
       <c r="F45" s="252" t="n">
-        <v>0.011428573168814182</v>
+        <v>0.0035714288242161274</v>
       </c>
       <c r="G45" s="252" t="n">
-        <v>2.2222040053138475E-4</v>
+        <v>6.944386950702684E-5</v>
       </c>
       <c r="H45" s="253" t="n">
-        <v>399.99672095649254</v>
+        <v>124.9989651126483</v>
       </c>
       <c r="I45" s="253" t="n">
-        <v>5.633756633190035E-4</v>
-      </c>
-      <c r="J45" s="253" t="s">
-        <v>249</v>
-      </c>
-      <c r="K45" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="L45" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="M45" s="253" t="s">
-        <v>249</v>
-      </c>
-      <c r="N45" s="273"/>
+        <v>1.8518365201873824E-4</v>
+      </c>
+      <c r="J45" s="253" t="n">
+        <v>0.0035714288242161274</v>
+      </c>
+      <c r="K45" s="252" t="n">
+        <v>6.944444612599909E-5</v>
+      </c>
+      <c r="L45" s="252" t="n">
+        <v>125.0</v>
+      </c>
+      <c r="M45" s="253" t="n">
+        <v>0.0011947432067245245</v>
+      </c>
+      <c r="N45" s="425" t="s">
+        <v>59</v>
+      </c>
       <c r="O45" s="64"/>
       <c r="P45" s="232"/>
       <c r="Q45" s="243" t="s">
         <v>247</v>
       </c>
       <c r="R45" s="381" t="s">
-        <v>224</v>
+        <v>251</v>
       </c>
       <c r="S45" s="381" t="n">
-        <v>300000.0</v>
+        <v>55000.0</v>
       </c>
       <c r="T45" s="381" t="n">
-        <v>40.0</v>
+        <v>70.0</v>
       </c>
       <c r="U45" s="381" t="n">
-        <v>10.0</v>
+        <v>120.0</v>
       </c>
       <c r="V45" s="381" t="n">
-        <v>50.0</v>
+        <v>100.0</v>
       </c>
       <c r="W45" s="381" t="n">
-        <v>8.757527684792876E-4</v>
+        <v>0.008296363987028599</v>
       </c>
       <c r="X45" s="381" t="n">
-        <v>8.757527684792877E-5</v>
+        <v>6.913636655857166E-5</v>
       </c>
       <c r="Y45" s="382" t="n">
-        <v>1.313629181822762E-4</v>
+        <v>6.518571899505332E-5</v>
       </c>
       <c r="Z45" s="381" t="n">
-        <v>8.757527102716267E-4</v>
+        <v>0.05352449789643288</v>
       </c>
       <c r="AA45" s="381" t="n">
-        <v>8.757527393754572E-5</v>
+        <v>4.460374766495079E-4</v>
       </c>
       <c r="AB45" s="383" t="n">
-        <v>1.3136290363036096E-4</v>
+        <v>4.205496225040406E-4</v>
       </c>
       <c r="AC45" s="405" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD45" s="64"/>
       <c r="AE45" s="50"/>
@@ -11273,49 +11265,57 @@
       <c r="A46" s="276"/>
       <c r="B46" s="276"/>
       <c r="D46" s="34"/>
-      <c r="E46" s="34" t="s">
-        <v>250</v>
-      </c>
-      <c r="F46" s="252" t="n">
-        <v>0.011428573168814182</v>
-      </c>
-      <c r="G46" s="252" t="n">
-        <v>3.1746036580039396E-5</v>
-      </c>
-      <c r="H46" s="253" t="n">
-        <v>31.746036580039398</v>
-      </c>
-      <c r="I46" s="253" t="n">
-        <v>7.297939443687218E-5</v>
-      </c>
-      <c r="J46" s="253" t="s">
-        <v>249</v>
-      </c>
-      <c r="K46" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="L46" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="M46" s="253" t="s">
-        <v>249</v>
-      </c>
+      <c r="E46" s="34"/>
+      <c r="F46" s="252"/>
+      <c r="G46" s="252"/>
+      <c r="H46" s="253"/>
+      <c r="I46" s="253"/>
+      <c r="J46" s="253"/>
+      <c r="K46" s="252"/>
+      <c r="L46" s="252"/>
+      <c r="M46" s="253"/>
       <c r="N46" s="301"/>
       <c r="O46" s="64"/>
       <c r="P46" s="232"/>
-      <c r="Q46" s="243"/>
-      <c r="R46" s="381"/>
-      <c r="S46" s="381"/>
-      <c r="T46" s="381"/>
-      <c r="U46" s="381"/>
-      <c r="V46" s="381"/>
-      <c r="W46" s="381"/>
-      <c r="X46" s="381"/>
-      <c r="Y46" s="382"/>
-      <c r="Z46" s="381"/>
-      <c r="AA46" s="381"/>
-      <c r="AB46" s="383"/>
-      <c r="AC46" s="384"/>
+      <c r="Q46" s="243" t="s">
+        <v>247</v>
+      </c>
+      <c r="R46" s="381" t="s">
+        <v>222</v>
+      </c>
+      <c r="S46" s="381" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="T46" s="381" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="U46" s="381" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="V46" s="381" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="W46" s="381" t="n">
+        <v>0.0023703896440565586</v>
+      </c>
+      <c r="X46" s="381" t="n">
+        <v>4.7407792881131175E-5</v>
+      </c>
+      <c r="Y46" s="382" t="n">
+        <v>3.9506496977992356E-4</v>
+      </c>
+      <c r="Z46" s="381" t="n">
+        <v>0.015292714349925518</v>
+      </c>
+      <c r="AA46" s="381" t="n">
+        <v>3.0585427884943783E-4</v>
+      </c>
+      <c r="AB46" s="383" t="n">
+        <v>0.002548785647377372</v>
+      </c>
+      <c r="AC46" s="406" t="s">
+        <v>59</v>
+      </c>
       <c r="AD46" s="64"/>
       <c r="AE46" s="50"/>
       <c r="AF46" s="50"/>
@@ -11333,75 +11333,55 @@
       <c r="A47" s="276"/>
       <c r="B47" s="276"/>
       <c r="D47" s="34"/>
-      <c r="E47" s="34" t="s">
-        <v>251</v>
-      </c>
-      <c r="F47" s="252" t="n">
-        <v>0.011428573168814182</v>
-      </c>
-      <c r="G47" s="252" t="n">
-        <v>1.5873018290019698E-5</v>
-      </c>
-      <c r="H47" s="252" t="n">
-        <v>19.04762194802364</v>
-      </c>
-      <c r="I47" s="252" t="n">
-        <v>4.378763666212331E-5</v>
-      </c>
-      <c r="J47" s="253" t="n">
-        <v>0.011428573168814182</v>
-      </c>
-      <c r="K47" s="252" t="n">
-        <v>1.587301812833175E-5</v>
-      </c>
-      <c r="L47" s="252" t="n">
-        <v>19.047622680664062</v>
-      </c>
-      <c r="M47" s="252" t="n">
-        <v>4.378763696877286E-5</v>
-      </c>
-      <c r="N47" s="406" t="s">
-        <v>56</v>
-      </c>
+      <c r="E47" s="34"/>
+      <c r="F47" s="252"/>
+      <c r="G47" s="252"/>
+      <c r="H47" s="252"/>
+      <c r="I47" s="252"/>
+      <c r="J47" s="253"/>
+      <c r="K47" s="252"/>
+      <c r="L47" s="252"/>
+      <c r="M47" s="252"/>
+      <c r="N47" s="274"/>
       <c r="P47" s="218"/>
       <c r="Q47" s="241" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="R47" s="382" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="S47" s="386" t="n">
-        <v>35000.0</v>
+        <v>15000.0</v>
       </c>
       <c r="T47" s="386" t="n">
-        <v>60.0</v>
+        <v>30.0</v>
       </c>
       <c r="U47" s="381" t="n">
-        <v>30.0</v>
+        <v>40.0</v>
       </c>
       <c r="V47" s="381" t="n">
-        <v>70.0</v>
+        <v>40.0</v>
       </c>
       <c r="W47" s="382" t="n">
-        <v>0.002627258189022541</v>
+        <v>0.003555584466084838</v>
       </c>
       <c r="X47" s="382" t="n">
-        <v>8.757527296741804E-5</v>
+        <v>8.888961165212094E-5</v>
       </c>
       <c r="Y47" s="382" t="n">
-        <v>2.189381848438643E-5</v>
+        <v>4.444480873644352E-5</v>
       </c>
       <c r="Z47" s="382" t="n">
-        <v>0.002627258189022541</v>
+        <v>0.02293907105922699</v>
       </c>
       <c r="AA47" s="382" t="n">
-        <v>8.757527393754572E-5</v>
+        <v>5.734767764806747E-4</v>
       </c>
       <c r="AB47" s="387" t="n">
-        <v>2.189381848438643E-5</v>
+        <v>2.8673838824033737E-4</v>
       </c>
       <c r="AC47" s="407" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD47" s="23"/>
       <c r="AE47" s="72"/>
@@ -11419,76 +11399,56 @@
     <row customHeight="1" ht="24.95" r="48" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A48" s="276"/>
       <c r="B48" s="276"/>
-      <c r="D48" s="34" t="s">
-        <v>255</v>
-      </c>
-      <c r="E48" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="F48" s="252" t="n">
-        <v>0.010000000707805157</v>
-      </c>
-      <c r="G48" s="252" t="n">
-        <v>1.9444283461967515E-4</v>
-      </c>
-      <c r="H48" s="252" t="n">
-        <v>349.99710231541525</v>
-      </c>
-      <c r="I48" s="252" t="n">
-        <v>8.045910398055523E-4</v>
-      </c>
-      <c r="J48" s="253" t="s">
-        <v>249</v>
-      </c>
-      <c r="K48" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="L48" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="M48" s="252" t="s">
-        <v>249</v>
-      </c>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="252"/>
+      <c r="G48" s="252"/>
+      <c r="H48" s="252"/>
+      <c r="I48" s="252"/>
+      <c r="J48" s="253"/>
+      <c r="K48" s="252"/>
+      <c r="L48" s="252"/>
+      <c r="M48" s="252"/>
       <c r="N48" s="274"/>
       <c r="P48" s="218"/>
       <c r="Q48" s="241" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="R48" s="382" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="S48" s="386" t="n">
-        <v>75000.0</v>
+        <v>300000.0</v>
       </c>
       <c r="T48" s="386" t="n">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c r="U48" s="381" t="n">
-        <v>100.0</v>
+        <v>10.0</v>
       </c>
       <c r="V48" s="381" t="n">
-        <v>30.0</v>
+        <v>50.0</v>
       </c>
       <c r="W48" s="382" t="n">
-        <v>0.002627258189022541</v>
+        <v>0.004740779288113117</v>
       </c>
       <c r="X48" s="382" t="n">
-        <v>2.627258189022541E-5</v>
+        <v>4.740779288113117E-4</v>
       </c>
       <c r="Y48" s="382" t="n">
-        <v>1.0946909605991095E-4</v>
+        <v>7.111169397830963E-4</v>
       </c>
       <c r="Z48" s="382" t="n">
-        <v>0.002627258189022541</v>
+        <v>0.030585428699851036</v>
       </c>
       <c r="AA48" s="382" t="n">
-        <v>2.6272582545061596E-5</v>
+        <v>0.0030585427302867174</v>
       </c>
       <c r="AB48" s="387" t="n">
-        <v>1.0946908878395334E-4</v>
+        <v>0.004587814211845398</v>
       </c>
       <c r="AC48" s="408" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD48" s="23"/>
       <c r="AE48" s="72"/>
@@ -11507,74 +11467,30 @@
       <c r="A49" s="276"/>
       <c r="B49" s="276"/>
       <c r="D49" s="34"/>
-      <c r="E49" s="34" t="s">
-        <v>250</v>
-      </c>
-      <c r="F49" s="252" t="n">
-        <v>0.010000000707805157</v>
-      </c>
-      <c r="G49" s="252" t="n">
-        <v>2.7777779743903213E-5</v>
-      </c>
-      <c r="H49" s="252" t="n">
-        <v>27.777779743903213</v>
-      </c>
-      <c r="I49" s="252" t="n">
-        <v>6.038647770413742E-5</v>
-      </c>
-      <c r="J49" s="253" t="s">
-        <v>249</v>
-      </c>
-      <c r="K49" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="L49" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="M49" s="252" t="s">
-        <v>249</v>
-      </c>
+      <c r="E49" s="34"/>
+      <c r="F49" s="252"/>
+      <c r="G49" s="252"/>
+      <c r="H49" s="252"/>
+      <c r="I49" s="252"/>
+      <c r="J49" s="253"/>
+      <c r="K49" s="252"/>
+      <c r="L49" s="252"/>
+      <c r="M49" s="252"/>
       <c r="N49" s="304"/>
       <c r="P49" s="218"/>
-      <c r="Q49" s="241" t="s">
-        <v>254</v>
-      </c>
-      <c r="R49" s="382" t="s">
-        <v>222</v>
-      </c>
-      <c r="S49" s="386" t="n">
-        <v>100000.0</v>
-      </c>
-      <c r="T49" s="386" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="U49" s="381" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="V49" s="381" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="W49" s="382" t="n">
-        <v>8.757527684792876E-4</v>
-      </c>
-      <c r="X49" s="382" t="n">
-        <v>1.751505536958575E-5</v>
-      </c>
-      <c r="Y49" s="382" t="n">
-        <v>1.4595879474654794E-4</v>
-      </c>
-      <c r="Z49" s="382" t="n">
-        <v>8.757527102716267E-4</v>
-      </c>
-      <c r="AA49" s="382" t="n">
-        <v>1.7515054423711263E-5</v>
-      </c>
-      <c r="AB49" s="387" t="n">
-        <v>1.4595879474654794E-4</v>
-      </c>
-      <c r="AC49" s="409" t="s">
-        <v>56</v>
-      </c>
+      <c r="Q49" s="241"/>
+      <c r="R49" s="382"/>
+      <c r="S49" s="386"/>
+      <c r="T49" s="386"/>
+      <c r="U49" s="381"/>
+      <c r="V49" s="381"/>
+      <c r="W49" s="382"/>
+      <c r="X49" s="382"/>
+      <c r="Y49" s="382"/>
+      <c r="Z49" s="382"/>
+      <c r="AA49" s="382"/>
+      <c r="AB49" s="387"/>
+      <c r="AC49" s="384"/>
       <c r="AD49" s="23"/>
       <c r="AE49" s="72"/>
       <c r="AF49" s="36"/>
@@ -11592,75 +11508,55 @@
       <c r="A50" s="276"/>
       <c r="B50" s="276"/>
       <c r="D50" s="34"/>
-      <c r="E50" s="34" t="s">
-        <v>251</v>
-      </c>
-      <c r="F50" s="252" t="n">
-        <v>0.010000000707805157</v>
-      </c>
-      <c r="G50" s="252" t="n">
-        <v>1.3888889871951606E-5</v>
-      </c>
-      <c r="H50" s="252" t="n">
-        <v>16.666667846341927</v>
-      </c>
-      <c r="I50" s="252" t="n">
-        <v>3.623188662248245E-5</v>
-      </c>
-      <c r="J50" s="252" t="n">
-        <v>0.010000000707805157</v>
-      </c>
-      <c r="K50" s="252" t="n">
-        <v>1.388888995279558E-5</v>
-      </c>
-      <c r="L50" s="252" t="n">
-        <v>16.666667938232422</v>
-      </c>
-      <c r="M50" s="252" t="n">
-        <v>3.6231886042514816E-5</v>
-      </c>
-      <c r="N50" s="411" t="s">
-        <v>56</v>
-      </c>
+      <c r="E50" s="34"/>
+      <c r="F50" s="252"/>
+      <c r="G50" s="252"/>
+      <c r="H50" s="252"/>
+      <c r="I50" s="252"/>
+      <c r="J50" s="252"/>
+      <c r="K50" s="252"/>
+      <c r="L50" s="252"/>
+      <c r="M50" s="252"/>
+      <c r="N50" s="274"/>
       <c r="P50" s="218"/>
       <c r="Q50" s="241" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="R50" s="382" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="S50" s="386" t="n">
-        <v>300000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="T50" s="386" t="n">
-        <v>40.0</v>
+        <v>50.0</v>
       </c>
       <c r="U50" s="381" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="V50" s="381" t="n">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c r="W50" s="382" t="n">
-        <v>0.0017515055369585752</v>
+        <v>0.01185194868594408</v>
       </c>
       <c r="X50" s="381" t="n">
-        <v>1.7515055369585753E-4</v>
+        <v>5.92597434297204E-4</v>
       </c>
       <c r="Y50" s="381" t="n">
-        <v>2.627258363645524E-4</v>
+        <v>3.9506496250396594E-5</v>
       </c>
       <c r="Z50" s="381" t="n">
-        <v>0.0017515054205432534</v>
+        <v>0.07646357268095016</v>
       </c>
       <c r="AA50" s="381" t="n">
-        <v>1.7515054787509143E-4</v>
+        <v>0.0038231785874813795</v>
       </c>
       <c r="AB50" s="383" t="n">
-        <v>2.627258072607219E-4</v>
+        <v>2.5487857055850327E-4</v>
       </c>
       <c r="AC50" s="410" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD50" s="46"/>
       <c r="AE50" s="50"/>
@@ -11678,51 +11574,57 @@
     <row customHeight="1" ht="24.95" r="51" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A51" s="276"/>
       <c r="B51" s="276"/>
-      <c r="D51" s="34" t="s">
-        <v>256</v>
-      </c>
-      <c r="E51" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="F51" s="252" t="n">
-        <v>0.019999999552965164</v>
-      </c>
-      <c r="G51" s="252" t="n">
-        <v>3.888856330215526E-4</v>
-      </c>
-      <c r="H51" s="252" t="n">
-        <v>699.9941394387947</v>
-      </c>
-      <c r="I51" s="252" t="n">
-        <v>0.0016091819297443556</v>
-      </c>
-      <c r="J51" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="K51" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="L51" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="M51" s="252" t="s">
-        <v>249</v>
-      </c>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="252"/>
+      <c r="G51" s="252"/>
+      <c r="H51" s="252"/>
+      <c r="I51" s="252"/>
+      <c r="J51" s="252"/>
+      <c r="K51" s="252"/>
+      <c r="L51" s="252"/>
+      <c r="M51" s="252"/>
       <c r="N51" s="274"/>
       <c r="P51" s="218"/>
-      <c r="Q51" s="241"/>
-      <c r="R51" s="382"/>
-      <c r="S51" s="386"/>
-      <c r="T51" s="386"/>
-      <c r="U51" s="381"/>
-      <c r="V51" s="381"/>
-      <c r="W51" s="382"/>
-      <c r="X51" s="381"/>
-      <c r="Y51" s="381"/>
-      <c r="Z51" s="381"/>
-      <c r="AA51" s="381"/>
-      <c r="AB51" s="383"/>
-      <c r="AC51" s="385"/>
+      <c r="Q51" s="241" t="s">
+        <v>252</v>
+      </c>
+      <c r="R51" s="382" t="s">
+        <v>249</v>
+      </c>
+      <c r="S51" s="386" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="T51" s="386" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="U51" s="381" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="V51" s="381" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="W51" s="382" t="n">
+        <v>0.014222337864339352</v>
+      </c>
+      <c r="X51" s="381" t="n">
+        <v>3.5555844660848377E-4</v>
+      </c>
+      <c r="Y51" s="381" t="n">
+        <v>2.962987055070698E-4</v>
+      </c>
+      <c r="Z51" s="381" t="n">
+        <v>0.09175628423690796</v>
+      </c>
+      <c r="AA51" s="381" t="n">
+        <v>0.002293907105922699</v>
+      </c>
+      <c r="AB51" s="383" t="n">
+        <v>0.0019115892937406898</v>
+      </c>
+      <c r="AC51" s="411" t="s">
+        <v>59</v>
+      </c>
       <c r="AD51" s="76"/>
       <c r="AE51" s="50"/>
       <c r="AF51" s="50"/>
@@ -11740,73 +11642,55 @@
       <c r="A52" s="276"/>
       <c r="B52" s="276"/>
       <c r="D52" s="34"/>
-      <c r="E52" s="34" t="s">
-        <v>250</v>
-      </c>
-      <c r="F52" s="252" t="n">
-        <v>0.019999999552965164</v>
-      </c>
-      <c r="G52" s="252" t="n">
-        <v>5.5555554313792125E-5</v>
-      </c>
-      <c r="H52" s="252" t="n">
-        <v>55.55555431379212</v>
-      </c>
-      <c r="I52" s="252" t="n">
-        <v>1.2077294416041766E-4</v>
-      </c>
-      <c r="J52" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="K52" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="L52" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="M52" s="252" t="s">
-        <v>249</v>
-      </c>
+      <c r="E52" s="34"/>
+      <c r="F52" s="252"/>
+      <c r="G52" s="252"/>
+      <c r="H52" s="252"/>
+      <c r="I52" s="252"/>
+      <c r="J52" s="252"/>
+      <c r="K52" s="252"/>
+      <c r="L52" s="252"/>
+      <c r="M52" s="252"/>
       <c r="N52" s="274"/>
       <c r="P52" s="218"/>
       <c r="Q52" s="241" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R52" s="382" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="S52" s="386" t="n">
-        <v>10000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="T52" s="386" t="n">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c r="U52" s="381" t="n">
-        <v>20.0</v>
+        <v>100.0</v>
       </c>
       <c r="V52" s="381" t="n">
-        <v>60.0</v>
+        <v>30.0</v>
       </c>
       <c r="W52" s="382" t="n">
-        <v>0.001811594353057444</v>
+        <v>0.014222337864339352</v>
       </c>
       <c r="X52" s="382" t="n">
-        <v>9.05797176528722E-5</v>
+        <v>1.4222337864339352E-4</v>
       </c>
       <c r="Y52" s="382" t="n">
-        <v>6.03864782533492E-6</v>
+        <v>5.925974692218006E-4</v>
       </c>
       <c r="Z52" s="382" t="n">
-        <v>0.001811594353057444</v>
+        <v>0.09175628423690796</v>
       </c>
       <c r="AA52" s="382" t="n">
-        <v>9.057971328729764E-5</v>
+        <v>9.17562807444483E-4</v>
       </c>
       <c r="AB52" s="387" t="n">
-        <v>6.03864782533492E-6</v>
+        <v>0.0038231785874813795</v>
       </c>
       <c r="AC52" s="412" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD52" s="23"/>
       <c r="AE52" s="36"/>
@@ -11825,75 +11709,55 @@
       <c r="A53" s="276"/>
       <c r="B53" s="276"/>
       <c r="D53" s="34"/>
-      <c r="E53" s="34" t="s">
-        <v>251</v>
-      </c>
-      <c r="F53" s="252" t="n">
-        <v>0.019999999552965164</v>
-      </c>
-      <c r="G53" s="252" t="n">
-        <v>2.7777777156896063E-5</v>
-      </c>
-      <c r="H53" s="252" t="n">
-        <v>33.333332588275276</v>
-      </c>
-      <c r="I53" s="252" t="n">
-        <v>7.24637664962506E-5</v>
-      </c>
-      <c r="J53" s="252" t="n">
-        <v>0.019999999552965164</v>
-      </c>
-      <c r="K53" s="252" t="n">
-        <v>2.7777776267612353E-5</v>
-      </c>
-      <c r="L53" s="252" t="n">
-        <v>33.33333206176758</v>
-      </c>
-      <c r="M53" s="252" t="n">
-        <v>7.246376480907202E-5</v>
-      </c>
-      <c r="N53" s="417" t="s">
-        <v>56</v>
-      </c>
+      <c r="E53" s="34"/>
+      <c r="F53" s="252"/>
+      <c r="G53" s="252"/>
+      <c r="H53" s="252"/>
+      <c r="I53" s="252"/>
+      <c r="J53" s="252"/>
+      <c r="K53" s="252"/>
+      <c r="L53" s="252"/>
+      <c r="M53" s="252"/>
+      <c r="N53" s="307"/>
       <c r="P53" s="218"/>
       <c r="Q53" s="241" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R53" s="382" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="S53" s="386" t="n">
-        <v>35000.0</v>
+        <v>55000.0</v>
       </c>
       <c r="T53" s="386" t="n">
-        <v>60.0</v>
+        <v>70.0</v>
       </c>
       <c r="U53" s="381" t="n">
-        <v>30.0</v>
+        <v>120.0</v>
       </c>
       <c r="V53" s="381" t="n">
-        <v>70.0</v>
+        <v>100.0</v>
       </c>
       <c r="W53" s="382" t="n">
-        <v>0.002173913177102804</v>
+        <v>0.016592727974057198</v>
       </c>
       <c r="X53" s="382" t="n">
-        <v>7.246377257009347E-5</v>
+        <v>1.3827273311714332E-4</v>
       </c>
       <c r="Y53" s="382" t="n">
-        <v>1.8115943021257408E-5</v>
+        <v>1.3037143799010664E-4</v>
       </c>
       <c r="Z53" s="382" t="n">
-        <v>0.002173913177102804</v>
+        <v>0.10704899579286575</v>
       </c>
       <c r="AA53" s="382" t="n">
-        <v>7.246377208502963E-5</v>
+        <v>8.920749532990158E-4</v>
       </c>
       <c r="AB53" s="387" t="n">
-        <v>1.8115943021257408E-5</v>
+        <v>8.410992450080812E-4</v>
       </c>
       <c r="AC53" s="413" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD53" s="23"/>
       <c r="AE53" s="36"/>
@@ -11911,40 +11775,20 @@
     <row customHeight="1" ht="24.95" r="54" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A54" s="276"/>
       <c r="B54" s="276"/>
-      <c r="D54" s="34" t="s">
-        <v>257</v>
-      </c>
-      <c r="E54" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="F54" s="252" t="n">
-        <v>0.010000000707805157</v>
-      </c>
-      <c r="G54" s="252" t="n">
-        <v>1.9444283461967515E-4</v>
-      </c>
-      <c r="H54" s="252" t="n">
-        <v>349.99710231541525</v>
-      </c>
-      <c r="I54" s="252" t="n">
-        <v>8.045910398055523E-4</v>
-      </c>
-      <c r="J54" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="K54" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="L54" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="M54" s="252" t="s">
-        <v>249</v>
-      </c>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="252"/>
+      <c r="G54" s="252"/>
+      <c r="H54" s="252"/>
+      <c r="I54" s="252"/>
+      <c r="J54" s="252"/>
+      <c r="K54" s="252"/>
+      <c r="L54" s="252"/>
+      <c r="M54" s="252"/>
       <c r="N54" s="274"/>
       <c r="P54" s="218"/>
       <c r="Q54" s="241" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R54" s="382" t="s">
         <v>222</v>
@@ -11962,25 +11806,25 @@
         <v>30.0</v>
       </c>
       <c r="W54" s="382" t="n">
-        <v>7.246377062983811E-4</v>
+        <v>0.004740779288113117</v>
       </c>
       <c r="X54" s="382" t="n">
-        <v>1.4492754125967622E-5</v>
+        <v>9.481558576226235E-5</v>
       </c>
       <c r="Y54" s="382" t="n">
-        <v>1.2077295104973018E-4</v>
+        <v>7.901299395598471E-4</v>
       </c>
       <c r="Z54" s="382" t="n">
-        <v>7.246377062983811E-4</v>
+        <v>0.030585428699851036</v>
       </c>
       <c r="AA54" s="382" t="n">
-        <v>1.4492754417005926E-5</v>
+        <v>6.117085576988757E-4</v>
       </c>
       <c r="AB54" s="387" t="n">
-        <v>1.207729583256878E-4</v>
+        <v>0.005097571294754744</v>
       </c>
       <c r="AC54" s="414" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD54" s="23"/>
       <c r="AE54" s="36"/>
@@ -11999,39 +11843,19 @@
       <c r="A55" s="276"/>
       <c r="B55" s="276"/>
       <c r="D55" s="34"/>
-      <c r="E55" s="34" t="s">
-        <v>250</v>
-      </c>
-      <c r="F55" s="252" t="n">
-        <v>0.010000000707805157</v>
-      </c>
-      <c r="G55" s="252" t="n">
-        <v>2.7777779743903213E-5</v>
-      </c>
-      <c r="H55" s="252" t="n">
-        <v>27.777779743903213</v>
-      </c>
-      <c r="I55" s="252" t="n">
-        <v>6.038647770413742E-5</v>
-      </c>
-      <c r="J55" s="252" t="n">
-        <v>0.010000000707805157</v>
-      </c>
-      <c r="K55" s="252" t="n">
-        <v>2.777777990559116E-5</v>
-      </c>
-      <c r="L55" s="252" t="n">
-        <v>27.777780532836914</v>
-      </c>
-      <c r="M55" s="252" t="n">
-        <v>6.03864791628439E-5</v>
-      </c>
-      <c r="N55" s="423" t="s">
-        <v>56</v>
-      </c>
+      <c r="E55" s="34"/>
+      <c r="F55" s="252"/>
+      <c r="G55" s="252"/>
+      <c r="H55" s="252"/>
+      <c r="I55" s="252"/>
+      <c r="J55" s="252"/>
+      <c r="K55" s="252"/>
+      <c r="L55" s="252"/>
+      <c r="M55" s="252"/>
+      <c r="N55" s="274"/>
       <c r="P55" s="218"/>
       <c r="Q55" s="241" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R55" s="382" t="s">
         <v>223</v>
@@ -12049,25 +11873,25 @@
         <v>40.0</v>
       </c>
       <c r="W55" s="382" t="n">
-        <v>0.001086956588551402</v>
+        <v>0.007111168932169676</v>
       </c>
       <c r="X55" s="382" t="n">
-        <v>2.717391471378505E-5</v>
+        <v>1.7777922330424188E-4</v>
       </c>
       <c r="Y55" s="382" t="n">
-        <v>1.3586957720690407E-5</v>
+        <v>8.888961747288704E-5</v>
       </c>
       <c r="Z55" s="382" t="n">
-        <v>0.001086956588551402</v>
+        <v>0.04587814211845398</v>
       </c>
       <c r="AA55" s="382" t="n">
-        <v>2.7173915441380814E-5</v>
+        <v>0.0011469535529613495</v>
       </c>
       <c r="AB55" s="387" t="n">
-        <v>1.3586957720690407E-5</v>
+        <v>5.734767764806747E-4</v>
       </c>
       <c r="AC55" s="415" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD55" s="23"/>
       <c r="AE55" s="36"/>
@@ -12086,37 +11910,19 @@
       <c r="A56" s="276"/>
       <c r="B56" s="276"/>
       <c r="D56" s="34"/>
-      <c r="E56" s="34" t="s">
-        <v>251</v>
-      </c>
-      <c r="F56" s="252" t="n">
-        <v>0.010000000707805157</v>
-      </c>
-      <c r="G56" s="252" t="n">
-        <v>1.3888889871951606E-5</v>
-      </c>
-      <c r="H56" s="252" t="n">
-        <v>16.666667846341927</v>
-      </c>
-      <c r="I56" s="252" t="n">
-        <v>3.623188662248245E-5</v>
-      </c>
-      <c r="J56" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="K56" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="L56" s="252" t="s">
-        <v>249</v>
-      </c>
-      <c r="M56" s="252" t="s">
-        <v>249</v>
-      </c>
+      <c r="E56" s="34"/>
+      <c r="F56" s="252"/>
+      <c r="G56" s="252"/>
+      <c r="H56" s="252"/>
+      <c r="I56" s="252"/>
+      <c r="J56" s="252"/>
+      <c r="K56" s="252"/>
+      <c r="L56" s="252"/>
+      <c r="M56" s="252"/>
       <c r="N56" s="310"/>
       <c r="P56" s="218"/>
       <c r="Q56" s="241" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R56" s="382" t="s">
         <v>224</v>
@@ -12134,25 +11940,25 @@
         <v>50.0</v>
       </c>
       <c r="W56" s="382" t="n">
-        <v>0.0014492754125967622</v>
+        <v>0.009481558576226234</v>
       </c>
       <c r="X56" s="382" t="n">
-        <v>1.4492754125967623E-4</v>
+        <v>9.481558576226234E-4</v>
       </c>
       <c r="Y56" s="382" t="n">
-        <v>2.173913235310465E-4</v>
+        <v>0.0014222338795661926</v>
       </c>
       <c r="Z56" s="382" t="n">
-        <v>0.0014492754125967622</v>
+        <v>0.06117085739970207</v>
       </c>
       <c r="AA56" s="382" t="n">
-        <v>1.4492754417005926E-4</v>
+        <v>0.006117085460573435</v>
       </c>
       <c r="AB56" s="387" t="n">
-        <v>2.173913235310465E-4</v>
+        <v>0.009175628423690796</v>
       </c>
       <c r="AC56" s="416" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD56" s="23"/>
       <c r="AE56" s="36"/>
@@ -12170,36 +11976,16 @@
     <row customHeight="1" ht="24.95" r="57" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A57" s="276"/>
       <c r="B57" s="276"/>
-      <c r="D57" s="34" t="s">
-        <v>258</v>
-      </c>
-      <c r="E57" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="F57" s="239" t="n">
-        <v>0.015000000596046448</v>
-      </c>
-      <c r="G57" s="239" t="n">
-        <v>2.916642428750633E-4</v>
-      </c>
-      <c r="H57" s="239" t="n">
-        <v>524.9956371751139</v>
-      </c>
-      <c r="I57" s="239" t="n">
-        <v>0.001206886522241641</v>
-      </c>
-      <c r="J57" s="240" t="s">
-        <v>249</v>
-      </c>
-      <c r="K57" s="239" t="s">
-        <v>249</v>
-      </c>
-      <c r="L57" s="239" t="s">
-        <v>249</v>
-      </c>
-      <c r="M57" s="239" t="s">
-        <v>249</v>
-      </c>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="239"/>
+      <c r="G57" s="239"/>
+      <c r="H57" s="239"/>
+      <c r="I57" s="239"/>
+      <c r="J57" s="240"/>
+      <c r="K57" s="239"/>
+      <c r="L57" s="239"/>
+      <c r="M57" s="239"/>
       <c r="N57" s="275"/>
       <c r="P57" s="218"/>
       <c r="Q57" s="241"/>
@@ -12232,75 +12018,55 @@
       <c r="A58" s="276"/>
       <c r="B58" s="276"/>
       <c r="D58" s="34"/>
-      <c r="E58" s="34" t="s">
-        <v>250</v>
-      </c>
-      <c r="F58" s="239" t="n">
-        <v>0.015000000596046448</v>
-      </c>
-      <c r="G58" s="239" t="n">
-        <v>4.166666832235124E-5</v>
-      </c>
-      <c r="H58" s="239" t="n">
-        <v>41.66666832235124</v>
-      </c>
-      <c r="I58" s="239" t="n">
-        <v>9.057971374424182E-5</v>
-      </c>
-      <c r="J58" s="240" t="n">
-        <v>0.015000000596046448</v>
-      </c>
-      <c r="K58" s="239" t="n">
-        <v>4.166666985838674E-5</v>
-      </c>
-      <c r="L58" s="239" t="n">
-        <v>41.66666793823242</v>
-      </c>
-      <c r="M58" s="239" t="n">
-        <v>9.057971328729764E-5</v>
-      </c>
-      <c r="N58" s="429" t="s">
-        <v>56</v>
-      </c>
+      <c r="E58" s="34"/>
+      <c r="F58" s="239"/>
+      <c r="G58" s="239"/>
+      <c r="H58" s="239"/>
+      <c r="I58" s="239"/>
+      <c r="J58" s="240"/>
+      <c r="K58" s="239"/>
+      <c r="L58" s="239"/>
+      <c r="M58" s="239"/>
+      <c r="N58" s="275"/>
       <c r="P58" s="218"/>
       <c r="Q58" s="241" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="R58" s="382" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
       <c r="S58" s="386" t="n">
-        <v>10000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="T58" s="386" t="n">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c r="U58" s="382" t="n">
-        <v>20.0</v>
+        <v>30.0</v>
       </c>
       <c r="V58" s="382" t="n">
-        <v>60.0</v>
+        <v>70.0</v>
       </c>
       <c r="W58" s="382" t="n">
-        <v>0.003623188240453601</v>
+        <v>0.022222038358449936</v>
       </c>
       <c r="X58" s="382" t="n">
-        <v>1.8115941202268004E-4</v>
+        <v>7.407346119483311E-4</v>
       </c>
       <c r="Y58" s="382" t="n">
-        <v>1.2077293831680436E-5</v>
+        <v>1.8518365686759353E-4</v>
       </c>
       <c r="Z58" s="382" t="n">
-        <v>0.003623188240453601</v>
+        <v>0.1433691829442978</v>
       </c>
       <c r="AA58" s="382" t="n">
-        <v>1.8115941202268004E-4</v>
+        <v>0.004778972826898098</v>
       </c>
       <c r="AB58" s="387" t="n">
-        <v>1.2077294741175137E-5</v>
+        <v>0.0011947432067245245</v>
       </c>
       <c r="AC58" s="418" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD58" s="23"/>
       <c r="AE58" s="36"/>
@@ -12319,73 +12085,55 @@
       <c r="A59" s="276"/>
       <c r="B59" s="276"/>
       <c r="D59" s="34"/>
-      <c r="E59" s="34" t="s">
-        <v>251</v>
-      </c>
-      <c r="F59" s="239" t="n">
-        <v>0.015000000596046448</v>
-      </c>
-      <c r="G59" s="239" t="n">
-        <v>2.083333416117562E-5</v>
-      </c>
-      <c r="H59" s="239" t="n">
-        <v>25.000000993410744</v>
-      </c>
-      <c r="I59" s="239" t="n">
-        <v>5.434782824654509E-5</v>
-      </c>
-      <c r="J59" s="240" t="s">
-        <v>249</v>
-      </c>
-      <c r="K59" s="239" t="s">
-        <v>249</v>
-      </c>
-      <c r="L59" s="239" t="s">
-        <v>249</v>
-      </c>
-      <c r="M59" s="239" t="s">
-        <v>249</v>
-      </c>
+      <c r="E59" s="34"/>
+      <c r="F59" s="239"/>
+      <c r="G59" s="239"/>
+      <c r="H59" s="239"/>
+      <c r="I59" s="239"/>
+      <c r="J59" s="240"/>
+      <c r="K59" s="239"/>
+      <c r="L59" s="239"/>
+      <c r="M59" s="239"/>
       <c r="N59" s="239"/>
       <c r="P59" s="218"/>
       <c r="Q59" s="241" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="R59" s="382" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="S59" s="386" t="n">
-        <v>35000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="T59" s="386" t="n">
         <v>60.0</v>
       </c>
       <c r="U59" s="382" t="n">
-        <v>30.0</v>
+        <v>40.0</v>
       </c>
       <c r="V59" s="382" t="n">
-        <v>70.0</v>
+        <v>20.0</v>
       </c>
       <c r="W59" s="382" t="n">
-        <v>0.004347825888544321</v>
+        <v>0.022222038358449936</v>
       </c>
       <c r="X59" s="382" t="n">
-        <v>1.4492752961814404E-4</v>
+        <v>5.555509589612484E-4</v>
       </c>
       <c r="Y59" s="382" t="n">
-        <v>3.623188240453601E-5</v>
+        <v>4.629591421689838E-4</v>
       </c>
       <c r="Z59" s="382" t="n">
-        <v>0.004347825888544321</v>
+        <v>0.1433691829442978</v>
       </c>
       <c r="AA59" s="382" t="n">
-        <v>1.4492752961814404E-4</v>
+        <v>0.00358422938734293</v>
       </c>
       <c r="AB59" s="387" t="n">
-        <v>3.623188240453601E-5</v>
+        <v>0.0029868579003959894</v>
       </c>
       <c r="AC59" s="419" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD59" s="23"/>
       <c r="AE59" s="36"/>
@@ -12416,43 +12164,43 @@
       <c r="N60" s="239"/>
       <c r="P60" s="218"/>
       <c r="Q60" s="241" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="R60" s="382" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="S60" s="386" t="n">
-        <v>100000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="T60" s="386" t="n">
-        <v>20.0</v>
+        <v>60.0</v>
       </c>
       <c r="U60" s="382" t="n">
-        <v>50.0</v>
+        <v>100.0</v>
       </c>
       <c r="V60" s="382" t="n">
         <v>30.0</v>
       </c>
       <c r="W60" s="382" t="n">
-        <v>0.0014492752961814404</v>
+        <v>0.022222038358449936</v>
       </c>
       <c r="X60" s="382" t="n">
-        <v>2.8985505923628808E-5</v>
+        <v>2.2222038358449937E-4</v>
       </c>
       <c r="Y60" s="382" t="n">
-        <v>2.4154588754754514E-4</v>
+        <v>9.259182843379676E-4</v>
       </c>
       <c r="Z60" s="382" t="n">
-        <v>0.0014492752961814404</v>
+        <v>0.1433691829442978</v>
       </c>
       <c r="AA60" s="382" t="n">
-        <v>2.898550701502245E-5</v>
+        <v>0.001433691824786365</v>
       </c>
       <c r="AB60" s="387" t="n">
-        <v>2.4154588754754514E-4</v>
+        <v>0.005973715800791979</v>
       </c>
       <c r="AC60" s="420" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD60" s="23"/>
       <c r="AE60" s="36"/>
@@ -12481,43 +12229,43 @@
       <c r="N61" s="239"/>
       <c r="P61" s="218"/>
       <c r="Q61" s="241" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="R61" s="382" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
       <c r="S61" s="386" t="n">
-        <v>15000.0</v>
+        <v>55000.0</v>
       </c>
       <c r="T61" s="386" t="n">
-        <v>30.0</v>
+        <v>70.0</v>
       </c>
       <c r="U61" s="382" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="V61" s="382" t="n">
-        <v>40.0</v>
+        <v>100.0</v>
       </c>
       <c r="W61" s="382" t="n">
-        <v>0.0021739129442721605</v>
+        <v>0.025925712659955025</v>
       </c>
       <c r="X61" s="382" t="n">
-        <v>5.434782360680401E-5</v>
+        <v>2.160476054996252E-4</v>
       </c>
       <c r="Y61" s="382" t="n">
-        <v>2.7173911803402007E-5</v>
+        <v>2.0370203128550202E-4</v>
       </c>
       <c r="Z61" s="382" t="n">
-        <v>0.0021739129442721605</v>
+        <v>0.16726404428482056</v>
       </c>
       <c r="AA61" s="382" t="n">
-        <v>5.434782360680401E-5</v>
+        <v>0.0013938670745119452</v>
       </c>
       <c r="AB61" s="388" t="n">
-        <v>2.7173911803402007E-5</v>
+        <v>0.0013142174575477839</v>
       </c>
       <c r="AC61" s="421" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD61" s="23"/>
       <c r="AE61" s="36"/>
@@ -12546,43 +12294,43 @@
       <c r="N62" s="239"/>
       <c r="P62" s="218"/>
       <c r="Q62" s="241" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="R62" s="382" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="S62" s="386" t="n">
-        <v>300000.0</v>
+        <v>100000.0</v>
       </c>
       <c r="T62" s="386" t="n">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="U62" s="382" t="n">
-        <v>10.0</v>
+        <v>50.0</v>
       </c>
       <c r="V62" s="382" t="n">
-        <v>50.0</v>
+        <v>30.0</v>
       </c>
       <c r="W62" s="382" t="n">
-        <v>0.0028985505923628807</v>
+        <v>0.007407346274703741</v>
       </c>
       <c r="X62" s="382" t="n">
-        <v>2.8985505923628807E-4</v>
+        <v>1.481469254940748E-4</v>
       </c>
       <c r="Y62" s="382" t="n">
-        <v>4.347825888544321E-4</v>
+        <v>0.0012345577124506235</v>
       </c>
       <c r="Z62" s="382" t="n">
-        <v>0.0028985505923628807</v>
+        <v>0.04778972640633583</v>
       </c>
       <c r="AA62" s="382" t="n">
-        <v>2.8985505923628807E-4</v>
+        <v>9.55794530455023E-4</v>
       </c>
       <c r="AB62" s="388" t="n">
-        <v>4.347825888544321E-4</v>
+        <v>0.00796495471149683</v>
       </c>
       <c r="AC62" s="422" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AD62" s="23"/>
       <c r="AE62" s="36"/>
@@ -12610,19 +12358,45 @@
       <c r="M63" s="239"/>
       <c r="N63" s="239"/>
       <c r="P63" s="218"/>
-      <c r="Q63" s="241"/>
-      <c r="R63" s="382"/>
-      <c r="S63" s="386"/>
-      <c r="T63" s="386"/>
-      <c r="U63" s="382"/>
-      <c r="V63" s="382"/>
-      <c r="W63" s="382"/>
-      <c r="X63" s="382"/>
-      <c r="Y63" s="382"/>
-      <c r="Z63" s="382"/>
-      <c r="AA63" s="382"/>
-      <c r="AB63" s="388"/>
-      <c r="AC63" s="384"/>
+      <c r="Q63" s="241" t="s">
+        <v>253</v>
+      </c>
+      <c r="R63" s="382" t="s">
+        <v>223</v>
+      </c>
+      <c r="S63" s="386" t="n">
+        <v>15000.0</v>
+      </c>
+      <c r="T63" s="386" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="U63" s="382" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="V63" s="382" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="W63" s="382" t="n">
+        <v>0.011111019179224968</v>
+      </c>
+      <c r="X63" s="382" t="n">
+        <v>2.777754794806242E-4</v>
+      </c>
+      <c r="Y63" s="382" t="n">
+        <v>1.3888774265069515E-4</v>
+      </c>
+      <c r="Z63" s="382" t="n">
+        <v>0.0716845914721489</v>
+      </c>
+      <c r="AA63" s="382" t="n">
+        <v>0.001792114693671465</v>
+      </c>
+      <c r="AB63" s="388" t="n">
+        <v>8.960573468357325E-4</v>
+      </c>
+      <c r="AC63" s="423" t="s">
+        <v>59</v>
+      </c>
       <c r="AD63" s="23"/>
       <c r="AE63" s="36"/>
       <c r="AF63" s="36"/>
@@ -12650,40 +12424,40 @@
       <c r="N64" s="239"/>
       <c r="P64" s="218"/>
       <c r="Q64" s="82" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="R64" s="382" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S64" s="389" t="n">
-        <v>10000.0</v>
+        <v>300000.0</v>
       </c>
       <c r="T64" s="389" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="U64" s="382" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="V64" s="382" t="n">
         <v>50.0</v>
       </c>
-      <c r="U64" s="382" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="V64" s="382" t="n">
-        <v>60.0</v>
-      </c>
       <c r="W64" s="382" t="n">
-        <v>0.001811594353057444</v>
+        <v>0.014814692549407482</v>
       </c>
       <c r="X64" s="382" t="n">
-        <v>9.05797176528722E-5</v>
+        <v>0.0014814692549407482</v>
       </c>
       <c r="Y64" s="382" t="n">
-        <v>6.03864782533492E-6</v>
+        <v>0.0022222038824111223</v>
       </c>
       <c r="Z64" s="382" t="n">
-        <v>0.003019323805347085</v>
+        <v>0.09557945281267166</v>
       </c>
       <c r="AA64" s="382" t="n">
-        <v>1.5096619608812034E-4</v>
+        <v>0.009557945653796196</v>
       </c>
       <c r="AB64" s="388" t="n">
-        <v>1.0064412890642416E-5</v>
+        <v>0.01433691754937172</v>
       </c>
       <c r="AC64" s="424" t="s">
         <v>59</v>
@@ -12714,45 +12488,19 @@
       <c r="M65" s="239"/>
       <c r="N65" s="239"/>
       <c r="P65" s="218"/>
-      <c r="Q65" s="82" t="s">
-        <v>257</v>
-      </c>
-      <c r="R65" s="382" t="s">
-        <v>252</v>
-      </c>
-      <c r="S65" s="389" t="n">
-        <v>35000.0</v>
-      </c>
-      <c r="T65" s="389" t="n">
-        <v>60.0</v>
-      </c>
-      <c r="U65" s="382" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="V65" s="382" t="n">
-        <v>70.0</v>
-      </c>
-      <c r="W65" s="382" t="n">
-        <v>0.002173913177102804</v>
-      </c>
-      <c r="X65" s="382" t="n">
-        <v>7.246377257009347E-5</v>
-      </c>
-      <c r="Y65" s="382" t="n">
-        <v>1.8115943021257408E-5</v>
-      </c>
-      <c r="Z65" s="382" t="n">
-        <v>0.003623188706114888</v>
-      </c>
-      <c r="AA65" s="382" t="n">
-        <v>1.207729583256878E-4</v>
-      </c>
-      <c r="AB65" s="388" t="n">
-        <v>3.019323958142195E-5</v>
-      </c>
-      <c r="AC65" s="425" t="s">
-        <v>59</v>
-      </c>
+      <c r="Q65" s="82"/>
+      <c r="R65" s="382"/>
+      <c r="S65" s="389"/>
+      <c r="T65" s="389"/>
+      <c r="U65" s="382"/>
+      <c r="V65" s="382"/>
+      <c r="W65" s="382"/>
+      <c r="X65" s="382"/>
+      <c r="Y65" s="382"/>
+      <c r="Z65" s="382"/>
+      <c r="AA65" s="382"/>
+      <c r="AB65" s="388"/>
+      <c r="AC65" s="390"/>
       <c r="AE65" s="36"/>
       <c r="AF65" s="36"/>
       <c r="AG65" s="50"/>
@@ -12774,40 +12522,40 @@
       <c r="N66" s="239"/>
       <c r="P66" s="218"/>
       <c r="Q66" s="82" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R66" s="382" t="s">
-        <v>222</v>
+        <v>255</v>
       </c>
       <c r="S66" s="389" t="n">
-        <v>100000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="T66" s="389" t="n">
-        <v>20.0</v>
+        <v>60.0</v>
       </c>
       <c r="U66" s="382" t="n">
-        <v>50.0</v>
+        <v>30.0</v>
       </c>
       <c r="V66" s="382" t="n">
-        <v>30.0</v>
+        <v>70.0</v>
       </c>
       <c r="W66" s="382" t="n">
-        <v>7.246377062983811E-4</v>
+        <v>0.011111019179224968</v>
       </c>
       <c r="X66" s="382" t="n">
-        <v>1.4492754125967622E-5</v>
+        <v>3.703673059741656E-4</v>
       </c>
       <c r="Y66" s="382" t="n">
-        <v>1.2077295104973018E-4</v>
+        <v>9.259182843379676E-5</v>
       </c>
       <c r="Z66" s="382" t="n">
-        <v>0.0012077295687049627</v>
+        <v>0.0716845914721489</v>
       </c>
       <c r="AA66" s="382" t="n">
-        <v>2.415459130133968E-5</v>
+        <v>0.002389486413449049</v>
       </c>
       <c r="AB66" s="388" t="n">
-        <v>2.0128826145082712E-4</v>
+        <v>5.973716033622622E-4</v>
       </c>
       <c r="AC66" s="426" t="s">
         <v>59</v>
@@ -12833,40 +12581,40 @@
       <c r="N67" s="239"/>
       <c r="P67" s="218"/>
       <c r="Q67" s="82" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R67" s="382" t="s">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="S67" s="389" t="n">
-        <v>15000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="T67" s="389" t="n">
-        <v>30.0</v>
+        <v>60.0</v>
       </c>
       <c r="U67" s="382" t="n">
         <v>40.0</v>
       </c>
       <c r="V67" s="382" t="n">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="W67" s="382" t="n">
-        <v>0.001086956588551402</v>
+        <v>0.011111019179224968</v>
       </c>
       <c r="X67" s="382" t="n">
-        <v>2.717391471378505E-5</v>
+        <v>2.777754794806242E-4</v>
       </c>
       <c r="Y67" s="382" t="n">
-        <v>1.3586957720690407E-5</v>
+        <v>2.314795710844919E-4</v>
       </c>
       <c r="Z67" s="382" t="n">
-        <v>0.001811594353057444</v>
+        <v>0.0716845914721489</v>
       </c>
       <c r="AA67" s="382" t="n">
-        <v>4.528985664364882E-5</v>
+        <v>0.001792114693671465</v>
       </c>
       <c r="AB67" s="388" t="n">
-        <v>2.264492832182441E-5</v>
+        <v>0.0014934289501979947</v>
       </c>
       <c r="AC67" s="427" t="s">
         <v>59</v>
@@ -12892,40 +12640,40 @@
       <c r="N68" s="239"/>
       <c r="P68" s="218"/>
       <c r="Q68" s="82" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R68" s="382" t="s">
-        <v>224</v>
+        <v>250</v>
       </c>
       <c r="S68" s="389" t="n">
-        <v>300000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="T68" s="389" t="n">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c r="U68" s="382" t="n">
-        <v>10.0</v>
+        <v>100.0</v>
       </c>
       <c r="V68" s="382" t="n">
-        <v>50.0</v>
+        <v>30.0</v>
       </c>
       <c r="W68" s="382" t="n">
-        <v>0.0014492754125967622</v>
+        <v>0.011111019179224968</v>
       </c>
       <c r="X68" s="382" t="n">
-        <v>1.4492754125967623E-4</v>
+        <v>1.1111019179224968E-4</v>
       </c>
       <c r="Y68" s="382" t="n">
-        <v>2.173913235310465E-4</v>
+        <v>4.629591421689838E-4</v>
       </c>
       <c r="Z68" s="382" t="n">
-        <v>0.0024154591374099255</v>
+        <v>0.0716845914721489</v>
       </c>
       <c r="AA68" s="382" t="n">
-        <v>2.415459166513756E-4</v>
+        <v>7.168459123931825E-4</v>
       </c>
       <c r="AB68" s="388" t="n">
-        <v>3.6231885314919055E-4</v>
+        <v>0.0029868579003959894</v>
       </c>
       <c r="AC68" s="428" t="s">
         <v>59</v>
@@ -12950,19 +12698,45 @@
       <c r="M69" s="239"/>
       <c r="N69" s="239"/>
       <c r="P69" s="218"/>
-      <c r="Q69" s="82"/>
-      <c r="R69" s="382"/>
-      <c r="S69" s="389"/>
-      <c r="T69" s="389"/>
-      <c r="U69" s="382"/>
-      <c r="V69" s="382"/>
-      <c r="W69" s="382"/>
-      <c r="X69" s="382"/>
-      <c r="Y69" s="382"/>
-      <c r="Z69" s="382"/>
-      <c r="AA69" s="382"/>
-      <c r="AB69" s="388"/>
-      <c r="AC69" s="390"/>
+      <c r="Q69" s="82" t="s">
+        <v>256</v>
+      </c>
+      <c r="R69" s="382" t="s">
+        <v>251</v>
+      </c>
+      <c r="S69" s="389" t="n">
+        <v>55000.0</v>
+      </c>
+      <c r="T69" s="389" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="U69" s="382" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="V69" s="382" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="W69" s="382" t="n">
+        <v>0.012962856329977512</v>
+      </c>
+      <c r="X69" s="382" t="n">
+        <v>1.080238027498126E-4</v>
+      </c>
+      <c r="Y69" s="382" t="n">
+        <v>1.0185101564275101E-4</v>
+      </c>
+      <c r="Z69" s="382" t="n">
+        <v>0.08363202214241028</v>
+      </c>
+      <c r="AA69" s="382" t="n">
+        <v>6.969335372559726E-4</v>
+      </c>
+      <c r="AB69" s="388" t="n">
+        <v>6.571087287738919E-4</v>
+      </c>
+      <c r="AC69" s="429" t="s">
+        <v>59</v>
+      </c>
       <c r="AE69" s="36"/>
       <c r="AF69" s="36"/>
       <c r="AG69" s="50"/>
@@ -12984,40 +12758,40 @@
       <c r="N70" s="239"/>
       <c r="P70" s="218"/>
       <c r="Q70" s="82" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="R70" s="382" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="S70" s="389" t="n">
-        <v>10000.0</v>
+        <v>100000.0</v>
       </c>
       <c r="T70" s="389" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="U70" s="382" t="n">
         <v>50.0</v>
       </c>
-      <c r="U70" s="382" t="n">
-        <v>20.0</v>
-      </c>
       <c r="V70" s="382" t="n">
-        <v>60.0</v>
+        <v>30.0</v>
       </c>
       <c r="W70" s="382" t="n">
-        <v>0.0027173913549631834</v>
+        <v>0.0037036731373518705</v>
       </c>
       <c r="X70" s="382" t="n">
-        <v>1.3586956774815916E-4</v>
+        <v>7.40734627470374E-5</v>
       </c>
       <c r="Y70" s="382" t="n">
-        <v>9.057970601134002E-6</v>
+        <v>6.172788562253118E-4</v>
       </c>
       <c r="Z70" s="382" t="n">
-        <v>0.004528985824435949</v>
+        <v>0.023894863203167915</v>
       </c>
       <c r="AA70" s="382" t="n">
-        <v>2.2644927958026528E-4</v>
+        <v>4.778972652275115E-4</v>
       </c>
       <c r="AB70" s="388" t="n">
-        <v>1.5096618881216273E-5</v>
+        <v>0.003982477355748415</v>
       </c>
       <c r="AC70" s="430" t="s">
         <v>59</v>
@@ -13043,40 +12817,40 @@
       <c r="N71" s="239"/>
       <c r="P71" s="218"/>
       <c r="Q71" s="82" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="R71" s="382" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="S71" s="389" t="n">
-        <v>35000.0</v>
+        <v>15000.0</v>
       </c>
       <c r="T71" s="389" t="n">
-        <v>60.0</v>
+        <v>30.0</v>
       </c>
       <c r="U71" s="382" t="n">
-        <v>30.0</v>
+        <v>40.0</v>
       </c>
       <c r="V71" s="382" t="n">
-        <v>70.0</v>
+        <v>40.0</v>
       </c>
       <c r="W71" s="382" t="n">
-        <v>0.0032608695328235626</v>
+        <v>0.005555509589612484</v>
       </c>
       <c r="X71" s="382" t="n">
-        <v>1.0869565109411875E-4</v>
+        <v>1.388877397403121E-4</v>
       </c>
       <c r="Y71" s="382" t="n">
-        <v>2.717391362239141E-5</v>
+        <v>6.944387132534757E-5</v>
       </c>
       <c r="Z71" s="382" t="n">
-        <v>0.005434782709926367</v>
+        <v>0.03584229573607445</v>
       </c>
       <c r="AA71" s="382" t="n">
-        <v>1.8115942657459527E-4</v>
+        <v>8.960573468357325E-4</v>
       </c>
       <c r="AB71" s="388" t="n">
-        <v>4.528985664364882E-5</v>
+        <v>4.4802867341786623E-4</v>
       </c>
       <c r="AC71" s="431" t="s">
         <v>59</v>
@@ -13102,40 +12876,40 @@
       <c r="N72" s="239"/>
       <c r="P72" s="218"/>
       <c r="Q72" s="82" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="R72" s="382" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="S72" s="389" t="n">
-        <v>100000.0</v>
+        <v>300000.0</v>
       </c>
       <c r="T72" s="389" t="n">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="U72" s="382" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="V72" s="382" t="n">
         <v>50.0</v>
       </c>
-      <c r="V72" s="382" t="n">
-        <v>30.0</v>
-      </c>
       <c r="W72" s="382" t="n">
-        <v>0.001086956588551402</v>
+        <v>0.007407346274703741</v>
       </c>
       <c r="X72" s="382" t="n">
-        <v>2.1739131771028042E-5</v>
+        <v>7.407346274703741E-4</v>
       </c>
       <c r="Y72" s="382" t="n">
-        <v>1.8115941202268004E-4</v>
+        <v>0.0011111019412055612</v>
       </c>
       <c r="Z72" s="382" t="n">
-        <v>0.0018115942366421223</v>
+        <v>0.04778972640633583</v>
       </c>
       <c r="AA72" s="382" t="n">
-        <v>3.6231886042514816E-5</v>
+        <v>0.004778972826898098</v>
       </c>
       <c r="AB72" s="388" t="n">
-        <v>3.019323921762407E-4</v>
+        <v>0.00716845877468586</v>
       </c>
       <c r="AC72" s="432" t="s">
         <v>59</v>
@@ -13160,45 +12934,19 @@
       <c r="M73" s="239"/>
       <c r="N73" s="239"/>
       <c r="P73" s="218"/>
-      <c r="Q73" s="82" t="s">
-        <v>258</v>
-      </c>
-      <c r="R73" s="382" t="s">
-        <v>223</v>
-      </c>
-      <c r="S73" s="389" t="n">
-        <v>15000.0</v>
-      </c>
-      <c r="T73" s="389" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="U73" s="382" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="V73" s="382" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="W73" s="382" t="n">
-        <v>0.0016304347664117813</v>
-      </c>
-      <c r="X73" s="382" t="n">
-        <v>4.0760869160294534E-5</v>
-      </c>
-      <c r="Y73" s="382" t="n">
-        <v>2.038043567154091E-5</v>
-      </c>
-      <c r="Z73" s="382" t="n">
-        <v>0.0027173913549631834</v>
-      </c>
-      <c r="AA73" s="382" t="n">
-        <v>6.793478678446263E-5</v>
-      </c>
-      <c r="AB73" s="388" t="n">
-        <v>3.3967393392231315E-5</v>
-      </c>
-      <c r="AC73" s="433" t="s">
-        <v>59</v>
-      </c>
+      <c r="Q73" s="82"/>
+      <c r="R73" s="382"/>
+      <c r="S73" s="389"/>
+      <c r="T73" s="389"/>
+      <c r="U73" s="382"/>
+      <c r="V73" s="382"/>
+      <c r="W73" s="382"/>
+      <c r="X73" s="382"/>
+      <c r="Y73" s="382"/>
+      <c r="Z73" s="382"/>
+      <c r="AA73" s="382"/>
+      <c r="AB73" s="388"/>
+      <c r="AC73" s="390"/>
       <c r="AE73" s="36"/>
       <c r="AF73" s="36"/>
       <c r="AG73" s="50"/>
@@ -13221,45 +12969,19 @@
       <c r="M74" s="50"/>
       <c r="N74" s="50"/>
       <c r="P74" s="218"/>
-      <c r="Q74" s="82" t="s">
-        <v>258</v>
-      </c>
-      <c r="R74" s="382" t="s">
-        <v>224</v>
-      </c>
-      <c r="S74" s="389" t="n">
-        <v>300000.0</v>
-      </c>
-      <c r="T74" s="389" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="U74" s="382" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="V74" s="382" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="W74" s="382" t="n">
-        <v>0.002173913177102804</v>
-      </c>
-      <c r="X74" s="382" t="n">
-        <v>2.173913177102804E-4</v>
-      </c>
-      <c r="Y74" s="382" t="n">
-        <v>3.2608697074465454E-4</v>
-      </c>
-      <c r="Z74" s="382" t="n">
-        <v>0.0036231884732842445</v>
-      </c>
-      <c r="AA74" s="382" t="n">
-        <v>3.6231885314919055E-4</v>
-      </c>
-      <c r="AB74" s="388" t="n">
-        <v>5.43478294275701E-4</v>
-      </c>
-      <c r="AC74" s="434" t="s">
-        <v>59</v>
-      </c>
+      <c r="Q74" s="82"/>
+      <c r="R74" s="382"/>
+      <c r="S74" s="389"/>
+      <c r="T74" s="389"/>
+      <c r="U74" s="382"/>
+      <c r="V74" s="382"/>
+      <c r="W74" s="382"/>
+      <c r="X74" s="382"/>
+      <c r="Y74" s="382"/>
+      <c r="Z74" s="382"/>
+      <c r="AA74" s="382"/>
+      <c r="AB74" s="388"/>
+      <c r="AC74" s="390"/>
       <c r="AE74" s="36"/>
       <c r="AF74" s="36"/>
       <c r="AG74" s="50"/>

</xml_diff>

<commit_message>
residue cal - same solubility
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase_result.xlsx
+++ b/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase_result.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="240">
   <si>
     <t>Testcase_id</t>
   </si>
@@ -767,34 +767,34 @@
     <t>Equipment Group saved successfully</t>
   </si>
   <si>
-    <t>Diluent</t>
+    <t>Liquid Anull</t>
   </si>
   <si>
-    <t>S1</t>
+    <t>Liquid A</t>
   </si>
   <si>
-    <t/>
+    <t>Liquid B</t>
   </si>
   <si>
-    <t>S2</t>
+    <t>Fail</t>
   </si>
   <si>
-    <t>Pass</t>
+    <t>Liquid A null</t>
   </si>
   <si>
-    <t>E1</t>
+    <t>L6</t>
   </si>
   <si>
-    <t>E1,</t>
+    <t>L5</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>L</t>
   </si>
   <si>
-    <t>E2</t>
+    <t>Liquid Bnull</t>
   </si>
   <si>
-    <t>E2,E1,</t>
+    <t>Liquid B null</t>
   </si>
 </sst>
 </file>
@@ -802,7 +802,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="88" x14ac:knownFonts="1">
+  <fonts count="94" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1286,22 +1286,52 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="17"/>
+      <color indexed="10"/>
     </font>
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="17"/>
+      <color indexed="10"/>
     </font>
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="17"/>
+      <color indexed="10"/>
     </font>
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="17"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1479,7 +1509,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="273">
+  <cellXfs count="279">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -2090,6 +2120,12 @@
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -4387,67 +4423,33 @@
       <c r="B42" s="125" t="s">
         <v>124</v>
       </c>
-      <c r="D42" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>230</v>
-      </c>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
       <c r="F42" s="118"/>
       <c r="G42" s="118"/>
-      <c r="H42" s="119" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="I42" s="119" t="n">
-        <v>600000.0</v>
-      </c>
+      <c r="H42" s="119"/>
+      <c r="I42" s="119"/>
       <c r="J42" s="119"/>
       <c r="K42" s="118"/>
-      <c r="L42" s="118" t="s">
-        <v>232</v>
-      </c>
-      <c r="M42" s="119" t="s">
-        <v>232</v>
-      </c>
+      <c r="L42" s="118"/>
+      <c r="M42" s="119"/>
       <c r="N42" s="142"/>
       <c r="O42" s="42"/>
       <c r="P42" s="104"/>
-      <c r="Q42" s="111" t="s">
-        <v>231</v>
-      </c>
-      <c r="R42" s="152" t="s">
-        <v>235</v>
-      </c>
-      <c r="S42" s="152" t="n">
-        <v>1000.0</v>
-      </c>
+      <c r="Q42" s="111"/>
+      <c r="R42" s="152"/>
+      <c r="S42" s="152"/>
       <c r="T42" s="152"/>
-      <c r="U42" s="152" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="V42" s="153" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="W42" s="154" t="n">
-        <v>0.10000000149011612</v>
-      </c>
+      <c r="U42" s="152"/>
+      <c r="V42" s="153"/>
+      <c r="W42" s="154"/>
       <c r="X42" s="155"/>
       <c r="Y42" s="48"/>
-      <c r="Z42" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="AA42" s="42" t="s">
-        <v>236</v>
-      </c>
-      <c r="AB42" s="42" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="AC42" s="152" t="n">
-        <v>285.71429443359375</v>
-      </c>
-      <c r="AD42" s="154" t="s">
-        <v>237</v>
-      </c>
+      <c r="Z42" s="42"/>
+      <c r="AA42" s="42"/>
+      <c r="AB42" s="42"/>
+      <c r="AC42" s="152"/>
+      <c r="AD42" s="154"/>
       <c r="AE42" s="161"/>
       <c r="AF42" s="101"/>
       <c r="AG42" s="42"/>
@@ -4464,31 +4466,17 @@
         <v>125</v>
       </c>
       <c r="D43" s="27"/>
-      <c r="E43" s="27" t="s">
-        <v>233</v>
-      </c>
+      <c r="E43" s="27"/>
       <c r="F43" s="119"/>
       <c r="G43" s="118"/>
-      <c r="H43" s="119" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="I43" s="120" t="n">
-        <v>600000.0</v>
-      </c>
+      <c r="H43" s="119"/>
+      <c r="I43" s="120"/>
       <c r="J43" s="119"/>
       <c r="K43" s="118"/>
-      <c r="L43" s="118" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="M43" s="120" t="n">
-        <v>600000.0</v>
-      </c>
-      <c r="N43" s="269" t="s">
-        <v>234</v>
-      </c>
-      <c r="O43" s="270" t="s">
-        <v>234</v>
-      </c>
+      <c r="L43" s="118"/>
+      <c r="M43" s="120"/>
+      <c r="N43" s="207"/>
+      <c r="O43" s="42"/>
       <c r="P43" s="104"/>
       <c r="Q43" s="111"/>
       <c r="R43" s="152"/>
@@ -4499,21 +4487,11 @@
       <c r="W43" s="154"/>
       <c r="X43" s="155"/>
       <c r="Y43" s="48"/>
-      <c r="Z43" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="AA43" s="42" t="s">
-        <v>239</v>
-      </c>
-      <c r="AB43" s="42" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="AC43" s="152" t="n">
-        <v>145.7142791748047</v>
-      </c>
-      <c r="AD43" s="154" t="s">
-        <v>237</v>
-      </c>
+      <c r="Z43" s="42"/>
+      <c r="AA43" s="42"/>
+      <c r="AB43" s="42"/>
+      <c r="AC43" s="152"/>
+      <c r="AD43" s="154"/>
       <c r="AE43" s="162"/>
       <c r="AF43" s="101"/>
       <c r="AG43" s="42"/>
@@ -4538,25 +4516,13 @@
       <c r="N44" s="208"/>
       <c r="O44" s="42"/>
       <c r="P44" s="104"/>
-      <c r="Q44" s="111" t="s">
-        <v>233</v>
-      </c>
-      <c r="R44" s="152" t="s">
-        <v>235</v>
-      </c>
-      <c r="S44" s="152" t="n">
-        <v>1000.0</v>
-      </c>
+      <c r="Q44" s="111"/>
+      <c r="R44" s="152"/>
+      <c r="S44" s="152"/>
       <c r="T44" s="152"/>
-      <c r="U44" s="152" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="V44" s="153" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="W44" s="154" t="n">
-        <v>0.10000000149011612</v>
-      </c>
+      <c r="U44" s="152"/>
+      <c r="V44" s="153"/>
+      <c r="W44" s="154"/>
       <c r="X44" s="155"/>
       <c r="Y44" s="48"/>
       <c r="Z44" s="42"/>
@@ -4575,50 +4541,26 @@
     <row customHeight="1" ht="24.95" r="45" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A45" s="125"/>
       <c r="B45" s="125"/>
-      <c r="D45" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>230</v>
-      </c>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
       <c r="F45" s="118"/>
       <c r="G45" s="118"/>
-      <c r="H45" s="119" t="n">
-        <v>5100.0</v>
-      </c>
-      <c r="I45" s="119" t="n">
-        <v>306000.0</v>
-      </c>
+      <c r="H45" s="119"/>
+      <c r="I45" s="119"/>
       <c r="J45" s="119"/>
       <c r="K45" s="118"/>
-      <c r="L45" s="118" t="s">
-        <v>232</v>
-      </c>
-      <c r="M45" s="119" t="s">
-        <v>232</v>
-      </c>
+      <c r="L45" s="118"/>
+      <c r="M45" s="119"/>
       <c r="N45" s="208"/>
       <c r="O45" s="42"/>
       <c r="P45" s="104"/>
-      <c r="Q45" s="111" t="s">
-        <v>233</v>
-      </c>
-      <c r="R45" s="152" t="s">
-        <v>238</v>
-      </c>
-      <c r="S45" s="152" t="n">
-        <v>2000.0</v>
-      </c>
+      <c r="Q45" s="111"/>
+      <c r="R45" s="152"/>
+      <c r="S45" s="152"/>
       <c r="T45" s="152"/>
-      <c r="U45" s="152" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="V45" s="153" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="W45" s="154" t="n">
-        <v>0.10000000149011612</v>
-      </c>
+      <c r="U45" s="152"/>
+      <c r="V45" s="153"/>
+      <c r="W45" s="154"/>
       <c r="X45" s="156"/>
       <c r="Y45" s="48"/>
       <c r="Z45" s="42"/>
@@ -4638,31 +4580,17 @@
       <c r="A46" s="125"/>
       <c r="B46" s="125"/>
       <c r="D46" s="27"/>
-      <c r="E46" s="27" t="s">
-        <v>231</v>
-      </c>
+      <c r="E46" s="27"/>
       <c r="F46" s="118"/>
       <c r="G46" s="118"/>
-      <c r="H46" s="119" t="n">
-        <v>1700.0</v>
-      </c>
-      <c r="I46" s="119" t="n">
-        <v>102000.0</v>
-      </c>
+      <c r="H46" s="119"/>
+      <c r="I46" s="119"/>
       <c r="J46" s="119"/>
       <c r="K46" s="118"/>
-      <c r="L46" s="118" t="n">
-        <v>1700.0</v>
-      </c>
-      <c r="M46" s="119" t="n">
-        <v>102000.0</v>
-      </c>
-      <c r="N46" s="271" t="s">
-        <v>234</v>
-      </c>
-      <c r="O46" s="272" t="s">
-        <v>234</v>
-      </c>
+      <c r="L46" s="118"/>
+      <c r="M46" s="119"/>
+      <c r="N46" s="143"/>
+      <c r="O46" s="42"/>
       <c r="P46" s="104"/>
       <c r="Q46" s="111"/>
       <c r="R46" s="152"/>
@@ -27901,32 +27829,80 @@
       <c r="B42" s="125" t="s">
         <v>124</v>
       </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="118"/>
-      <c r="G42" s="118"/>
-      <c r="H42" s="119"/>
-      <c r="I42" s="119"/>
-      <c r="J42" s="119"/>
-      <c r="K42" s="118"/>
-      <c r="L42" s="118"/>
-      <c r="M42" s="119"/>
-      <c r="N42" s="142"/>
+      <c r="D42" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="F42" s="118" t="n">
+        <v>0.02499999850988388</v>
+      </c>
+      <c r="G42" s="118" t="n">
+        <v>2.499999850988388E-4</v>
+      </c>
+      <c r="H42" s="119" t="n">
+        <v>124.9999925494194</v>
+      </c>
+      <c r="I42" s="119" t="n">
+        <v>3.7878785621036184E-4</v>
+      </c>
+      <c r="J42" s="119" t="n">
+        <v>0.019999999552965164</v>
+      </c>
+      <c r="K42" s="118" t="n">
+        <v>1.9999999494757503E-4</v>
+      </c>
+      <c r="L42" s="118" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="M42" s="119" t="n">
+        <v>3.030303050763905E-4</v>
+      </c>
+      <c r="N42" s="269" t="s">
+        <v>233</v>
+      </c>
       <c r="O42" s="48"/>
       <c r="P42" s="104"/>
-      <c r="Q42" s="111"/>
-      <c r="R42" s="152"/>
-      <c r="S42" s="152"/>
-      <c r="T42" s="152"/>
-      <c r="U42" s="152"/>
-      <c r="V42" s="152"/>
-      <c r="W42" s="152"/>
-      <c r="X42" s="152"/>
-      <c r="Y42" s="153"/>
-      <c r="Z42" s="152"/>
-      <c r="AA42" s="152"/>
-      <c r="AB42" s="154"/>
-      <c r="AC42" s="155"/>
+      <c r="Q42" s="111" t="s">
+        <v>234</v>
+      </c>
+      <c r="R42" s="152" t="s">
+        <v>235</v>
+      </c>
+      <c r="S42" s="152" t="n">
+        <v>28000.0</v>
+      </c>
+      <c r="T42" s="152" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="U42" s="152" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="V42" s="152" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="W42" s="152" t="n">
+        <v>0.03787878667935729</v>
+      </c>
+      <c r="X42" s="152" t="n">
+        <v>7.575757335871458E-4</v>
+      </c>
+      <c r="Y42" s="153" t="n">
+        <v>3.0303028651646206E-4</v>
+      </c>
+      <c r="Z42" s="152" t="n">
+        <v>0.030303029343485832</v>
+      </c>
+      <c r="AA42" s="152" t="n">
+        <v>6.06060610152781E-4</v>
+      </c>
+      <c r="AB42" s="154" t="n">
+        <v>2.4242424115072936E-4</v>
+      </c>
+      <c r="AC42" s="270" t="s">
+        <v>233</v>
+      </c>
       <c r="AD42" s="48"/>
       <c r="AE42" s="42"/>
       <c r="AF42" s="42"/>
@@ -27935,10 +27911,18 @@
       <c r="AI42" s="154"/>
       <c r="AJ42" s="161"/>
       <c r="AK42" s="101"/>
-      <c r="AL42" s="42"/>
-      <c r="AM42" s="42"/>
-      <c r="AN42" s="29"/>
-      <c r="AO42" s="29"/>
+      <c r="AL42" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="AM42" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="AN42" s="29" t="n">
+        <v>3.787878667935729E-4</v>
+      </c>
+      <c r="AO42" s="29" t="n">
+        <v>0.3030303120613098</v>
+      </c>
       <c r="AP42" s="16"/>
     </row>
     <row customHeight="1" ht="24.95" r="43" spans="1:42" x14ac:dyDescent="0.4">
@@ -27948,32 +27932,80 @@
       <c r="B43" s="125" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="119"/>
-      <c r="G43" s="118"/>
-      <c r="H43" s="119"/>
-      <c r="I43" s="120"/>
-      <c r="J43" s="119"/>
-      <c r="K43" s="118"/>
-      <c r="L43" s="118"/>
-      <c r="M43" s="120"/>
-      <c r="N43" s="121"/>
+      <c r="D43" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="E43" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="F43" s="119" t="n">
+        <v>0.019999999552965164</v>
+      </c>
+      <c r="G43" s="118" t="n">
+        <v>1.9999999552965163E-4</v>
+      </c>
+      <c r="H43" s="119" t="n">
+        <v>99.99999776482582</v>
+      </c>
+      <c r="I43" s="120" t="n">
+        <v>3.0303029625704795E-4</v>
+      </c>
+      <c r="J43" s="119" t="n">
+        <v>0.02499999850988388</v>
+      </c>
+      <c r="K43" s="118" t="n">
+        <v>2.4999998277053237E-4</v>
+      </c>
+      <c r="L43" s="118" t="n">
+        <v>124.99999237060547</v>
+      </c>
+      <c r="M43" s="120" t="n">
+        <v>3.787878667935729E-4</v>
+      </c>
+      <c r="N43" s="274" t="s">
+        <v>233</v>
+      </c>
       <c r="O43" s="48"/>
       <c r="P43" s="104"/>
-      <c r="Q43" s="111"/>
-      <c r="R43" s="152"/>
-      <c r="S43" s="152"/>
-      <c r="T43" s="152"/>
-      <c r="U43" s="152"/>
-      <c r="V43" s="152"/>
-      <c r="W43" s="152"/>
-      <c r="X43" s="152"/>
-      <c r="Y43" s="153"/>
-      <c r="Z43" s="152"/>
-      <c r="AA43" s="152"/>
-      <c r="AB43" s="154"/>
-      <c r="AC43" s="155"/>
+      <c r="Q43" s="111" t="s">
+        <v>234</v>
+      </c>
+      <c r="R43" s="152" t="s">
+        <v>236</v>
+      </c>
+      <c r="S43" s="152" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="T43" s="152" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="U43" s="152" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="V43" s="152" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="W43" s="152" t="n">
+        <v>0.03787878667935729</v>
+      </c>
+      <c r="X43" s="152" t="n">
+        <v>7.575757335871458E-4</v>
+      </c>
+      <c r="Y43" s="153" t="n">
+        <v>0.0010822510855538505</v>
+      </c>
+      <c r="Z43" s="152" t="n">
+        <v>0.030303029343485832</v>
+      </c>
+      <c r="AA43" s="152" t="n">
+        <v>6.06060610152781E-4</v>
+      </c>
+      <c r="AB43" s="154" t="n">
+        <v>8.658008300699294E-4</v>
+      </c>
+      <c r="AC43" s="271" t="s">
+        <v>233</v>
+      </c>
       <c r="AD43" s="48"/>
       <c r="AE43" s="42"/>
       <c r="AF43" s="42"/>
@@ -27982,10 +28014,18 @@
       <c r="AI43" s="154"/>
       <c r="AJ43" s="162"/>
       <c r="AK43" s="101"/>
-      <c r="AL43" s="42"/>
-      <c r="AM43" s="42"/>
-      <c r="AN43" s="29"/>
-      <c r="AO43" s="29"/>
+      <c r="AL43" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="AM43" s="42" t="s">
+        <v>236</v>
+      </c>
+      <c r="AN43" s="29" t="n">
+        <v>3.787878667935729E-4</v>
+      </c>
+      <c r="AO43" s="29" t="n">
+        <v>0.3030303120613098</v>
+      </c>
       <c r="AP43" s="16"/>
     </row>
     <row customHeight="1" ht="24.75" r="44" spans="1:42" x14ac:dyDescent="0.4">
@@ -28004,19 +28044,45 @@
       <c r="N44" s="122"/>
       <c r="O44" s="48"/>
       <c r="P44" s="104"/>
-      <c r="Q44" s="111"/>
-      <c r="R44" s="152"/>
-      <c r="S44" s="152"/>
-      <c r="T44" s="152"/>
-      <c r="U44" s="152"/>
-      <c r="V44" s="152"/>
-      <c r="W44" s="152"/>
-      <c r="X44" s="152"/>
-      <c r="Y44" s="153"/>
-      <c r="Z44" s="152"/>
-      <c r="AA44" s="152"/>
-      <c r="AB44" s="154"/>
-      <c r="AC44" s="155"/>
+      <c r="Q44" s="111" t="s">
+        <v>234</v>
+      </c>
+      <c r="R44" s="152" t="s">
+        <v>237</v>
+      </c>
+      <c r="S44" s="152" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="T44" s="152" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="U44" s="152" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="V44" s="152" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="W44" s="152" t="n">
+        <v>0.03787878667935729</v>
+      </c>
+      <c r="X44" s="152" t="n">
+        <v>7.575757335871458E-4</v>
+      </c>
+      <c r="Y44" s="153" t="n">
+        <v>2.164502143859863E-5</v>
+      </c>
+      <c r="Z44" s="152" t="n">
+        <v>0.030303029343485832</v>
+      </c>
+      <c r="AA44" s="152" t="n">
+        <v>6.06060610152781E-4</v>
+      </c>
+      <c r="AB44" s="154" t="n">
+        <v>1.7316016965196468E-5</v>
+      </c>
+      <c r="AC44" s="272" t="s">
+        <v>233</v>
+      </c>
       <c r="AD44" s="48"/>
       <c r="AE44" s="42"/>
       <c r="AF44" s="42"/>
@@ -28025,10 +28091,18 @@
       <c r="AI44" s="154"/>
       <c r="AJ44" s="163"/>
       <c r="AK44" s="101"/>
-      <c r="AL44" s="42"/>
-      <c r="AM44" s="42"/>
-      <c r="AN44" s="29"/>
-      <c r="AO44" s="29"/>
+      <c r="AL44" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="AM44" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN44" s="29" t="n">
+        <v>3.787878667935729E-4</v>
+      </c>
+      <c r="AO44" s="29" t="n">
+        <v>0.3030303120613098</v>
+      </c>
       <c r="AP44" s="16"/>
     </row>
     <row customHeight="1" ht="24.95" r="45" spans="1:42" x14ac:dyDescent="0.4">
@@ -28047,19 +28121,45 @@
       <c r="N45" s="122"/>
       <c r="O45" s="48"/>
       <c r="P45" s="104"/>
-      <c r="Q45" s="111"/>
-      <c r="R45" s="152"/>
-      <c r="S45" s="152"/>
-      <c r="T45" s="152"/>
-      <c r="U45" s="152"/>
-      <c r="V45" s="152"/>
-      <c r="W45" s="152"/>
-      <c r="X45" s="152"/>
-      <c r="Y45" s="153"/>
-      <c r="Z45" s="152"/>
-      <c r="AA45" s="152"/>
-      <c r="AB45" s="154"/>
-      <c r="AC45" s="156"/>
+      <c r="Q45" s="111" t="s">
+        <v>234</v>
+      </c>
+      <c r="R45" s="152" t="s">
+        <v>88</v>
+      </c>
+      <c r="S45" s="152" t="n">
+        <v>50000.0</v>
+      </c>
+      <c r="T45" s="152" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="U45" s="152" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="V45" s="152" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="W45" s="152" t="n">
+        <v>0.03787878667935729</v>
+      </c>
+      <c r="X45" s="152" t="n">
+        <v>7.575757335871458E-4</v>
+      </c>
+      <c r="Y45" s="153" t="n">
+        <v>5.411255427769252E-4</v>
+      </c>
+      <c r="Z45" s="152" t="n">
+        <v>0.030303029343485832</v>
+      </c>
+      <c r="AA45" s="152" t="n">
+        <v>6.06060610152781E-4</v>
+      </c>
+      <c r="AB45" s="154" t="n">
+        <v>4.329004150349647E-4</v>
+      </c>
+      <c r="AC45" s="273" t="s">
+        <v>233</v>
+      </c>
       <c r="AD45" s="48"/>
       <c r="AE45" s="42"/>
       <c r="AF45" s="42"/>
@@ -28068,10 +28168,18 @@
       <c r="AI45" s="154"/>
       <c r="AJ45" s="164"/>
       <c r="AK45" s="101"/>
-      <c r="AL45" s="42"/>
-      <c r="AM45" s="42"/>
-      <c r="AN45" s="29"/>
-      <c r="AO45" s="29"/>
+      <c r="AL45" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="AM45" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN45" s="29" t="n">
+        <v>3.787878667935729E-4</v>
+      </c>
+      <c r="AO45" s="29" t="n">
+        <v>0.3030303120613098</v>
+      </c>
       <c r="AP45" s="16"/>
     </row>
     <row customHeight="1" ht="24.95" r="46" spans="1:42" x14ac:dyDescent="0.4">
@@ -28111,10 +28219,18 @@
       <c r="AI46" s="154"/>
       <c r="AJ46" s="165"/>
       <c r="AK46" s="101"/>
-      <c r="AL46" s="42"/>
-      <c r="AM46" s="42"/>
-      <c r="AN46" s="29"/>
-      <c r="AO46" s="29"/>
+      <c r="AL46" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="AM46" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="AN46" s="29" t="n">
+        <v>3.030303050763905E-4</v>
+      </c>
+      <c r="AO46" s="29" t="n">
+        <v>0.3030303120613098</v>
+      </c>
       <c r="AP46" s="16"/>
     </row>
     <row customHeight="1" ht="24.95" r="47" spans="1:42" x14ac:dyDescent="0.4">
@@ -28132,19 +28248,45 @@
       <c r="M47" s="120"/>
       <c r="N47" s="123"/>
       <c r="P47" s="100"/>
-      <c r="Q47" s="109"/>
-      <c r="R47" s="153"/>
-      <c r="S47" s="157"/>
-      <c r="T47" s="157"/>
-      <c r="U47" s="152"/>
-      <c r="V47" s="152"/>
-      <c r="W47" s="153"/>
-      <c r="X47" s="153"/>
-      <c r="Y47" s="153"/>
-      <c r="Z47" s="153"/>
-      <c r="AA47" s="153"/>
-      <c r="AB47" s="158"/>
-      <c r="AC47" s="155"/>
+      <c r="Q47" s="109" t="s">
+        <v>239</v>
+      </c>
+      <c r="R47" s="153" t="s">
+        <v>235</v>
+      </c>
+      <c r="S47" s="157" t="n">
+        <v>28000.0</v>
+      </c>
+      <c r="T47" s="157" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="U47" s="152" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="V47" s="152" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="W47" s="153" t="n">
+        <v>0.03030303050763905</v>
+      </c>
+      <c r="X47" s="153" t="n">
+        <v>6.06060610152781E-4</v>
+      </c>
+      <c r="Y47" s="153" t="n">
+        <v>2.4242425646100725E-4</v>
+      </c>
+      <c r="Z47" s="153" t="n">
+        <v>0.03787878528237343</v>
+      </c>
+      <c r="AA47" s="153" t="n">
+        <v>7.575757335871458E-4</v>
+      </c>
+      <c r="AB47" s="158" t="n">
+        <v>3.0303027597256005E-4</v>
+      </c>
+      <c r="AC47" s="275" t="s">
+        <v>233</v>
+      </c>
       <c r="AD47" s="16"/>
       <c r="AE47" s="55"/>
       <c r="AF47" s="29"/>
@@ -28153,10 +28295,18 @@
       <c r="AI47" s="158"/>
       <c r="AJ47" s="166"/>
       <c r="AK47" s="101"/>
-      <c r="AL47" s="55"/>
-      <c r="AM47" s="55"/>
-      <c r="AN47" s="29"/>
-      <c r="AO47" s="29"/>
+      <c r="AL47" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="AM47" s="55" t="s">
+        <v>236</v>
+      </c>
+      <c r="AN47" s="29" t="n">
+        <v>3.030303050763905E-4</v>
+      </c>
+      <c r="AO47" s="29" t="n">
+        <v>0.3030303120613098</v>
+      </c>
       <c r="AP47" s="16"/>
     </row>
     <row customHeight="1" ht="24.95" r="48" spans="1:42" x14ac:dyDescent="0.4">
@@ -28174,19 +28324,45 @@
       <c r="M48" s="119"/>
       <c r="N48" s="123"/>
       <c r="P48" s="100"/>
-      <c r="Q48" s="109"/>
-      <c r="R48" s="153"/>
-      <c r="S48" s="157"/>
-      <c r="T48" s="157"/>
-      <c r="U48" s="152"/>
-      <c r="V48" s="152"/>
-      <c r="W48" s="153"/>
-      <c r="X48" s="153"/>
-      <c r="Y48" s="153"/>
-      <c r="Z48" s="153"/>
-      <c r="AA48" s="153"/>
-      <c r="AB48" s="158"/>
-      <c r="AC48" s="155"/>
+      <c r="Q48" s="109" t="s">
+        <v>239</v>
+      </c>
+      <c r="R48" s="153" t="s">
+        <v>236</v>
+      </c>
+      <c r="S48" s="157" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="T48" s="157" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="U48" s="152" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="V48" s="152" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="W48" s="153" t="n">
+        <v>0.03030303050763905</v>
+      </c>
+      <c r="X48" s="153" t="n">
+        <v>6.06060610152781E-4</v>
+      </c>
+      <c r="Y48" s="153" t="n">
+        <v>8.658008575439453E-4</v>
+      </c>
+      <c r="Z48" s="153" t="n">
+        <v>0.03787878528237343</v>
+      </c>
+      <c r="AA48" s="153" t="n">
+        <v>7.575757335871458E-4</v>
+      </c>
+      <c r="AB48" s="158" t="n">
+        <v>0.0010822509648278356</v>
+      </c>
+      <c r="AC48" s="276" t="s">
+        <v>233</v>
+      </c>
       <c r="AD48" s="16"/>
       <c r="AE48" s="55"/>
       <c r="AF48" s="29"/>
@@ -28195,10 +28371,18 @@
       <c r="AI48" s="158"/>
       <c r="AJ48" s="167"/>
       <c r="AK48" s="101"/>
-      <c r="AL48" s="55"/>
-      <c r="AM48" s="55"/>
-      <c r="AN48" s="29"/>
-      <c r="AO48" s="29"/>
+      <c r="AL48" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="AM48" s="55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN48" s="29" t="n">
+        <v>3.030303050763905E-4</v>
+      </c>
+      <c r="AO48" s="29" t="n">
+        <v>0.3030303120613098</v>
+      </c>
       <c r="AP48" s="16"/>
     </row>
     <row customHeight="1" ht="24.95" r="49" spans="1:42" x14ac:dyDescent="0.4">
@@ -28216,19 +28400,45 @@
       <c r="M49" s="119"/>
       <c r="N49" s="144"/>
       <c r="P49" s="100"/>
-      <c r="Q49" s="109"/>
-      <c r="R49" s="153"/>
-      <c r="S49" s="157"/>
-      <c r="T49" s="157"/>
-      <c r="U49" s="152"/>
-      <c r="V49" s="152"/>
-      <c r="W49" s="153"/>
-      <c r="X49" s="153"/>
-      <c r="Y49" s="153"/>
-      <c r="Z49" s="153"/>
-      <c r="AA49" s="153"/>
-      <c r="AB49" s="158"/>
-      <c r="AC49" s="155"/>
+      <c r="Q49" s="109" t="s">
+        <v>239</v>
+      </c>
+      <c r="R49" s="153" t="s">
+        <v>237</v>
+      </c>
+      <c r="S49" s="157" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="T49" s="157" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="U49" s="152" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="V49" s="152" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="W49" s="153" t="n">
+        <v>0.03030303050763905</v>
+      </c>
+      <c r="X49" s="153" t="n">
+        <v>6.06060610152781E-4</v>
+      </c>
+      <c r="Y49" s="153" t="n">
+        <v>1.7316017832074845E-5</v>
+      </c>
+      <c r="Z49" s="153" t="n">
+        <v>0.03787878528237343</v>
+      </c>
+      <c r="AA49" s="153" t="n">
+        <v>7.575757335871458E-4</v>
+      </c>
+      <c r="AB49" s="158" t="n">
+        <v>2.1645020751748234E-5</v>
+      </c>
+      <c r="AC49" s="277" t="s">
+        <v>233</v>
+      </c>
       <c r="AD49" s="16"/>
       <c r="AE49" s="55"/>
       <c r="AF49" s="29"/>
@@ -28237,10 +28447,18 @@
       <c r="AI49" s="158"/>
       <c r="AJ49" s="168"/>
       <c r="AK49" s="101"/>
-      <c r="AL49" s="55"/>
-      <c r="AM49" s="55"/>
-      <c r="AN49" s="29"/>
-      <c r="AO49" s="29"/>
+      <c r="AL49" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="AM49" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN49" s="29" t="n">
+        <v>3.030303050763905E-4</v>
+      </c>
+      <c r="AO49" s="29" t="n">
+        <v>0.3030303120613098</v>
+      </c>
       <c r="AP49" s="16"/>
     </row>
     <row customHeight="1" ht="24.95" r="50" spans="1:42" x14ac:dyDescent="0.4">
@@ -28258,19 +28476,45 @@
       <c r="M50" s="119"/>
       <c r="N50" s="123"/>
       <c r="P50" s="100"/>
-      <c r="Q50" s="109"/>
-      <c r="R50" s="153"/>
-      <c r="S50" s="157"/>
-      <c r="T50" s="157"/>
-      <c r="U50" s="152"/>
-      <c r="V50" s="152"/>
-      <c r="W50" s="153"/>
-      <c r="X50" s="152"/>
-      <c r="Y50" s="152"/>
-      <c r="Z50" s="152"/>
-      <c r="AA50" s="152"/>
-      <c r="AB50" s="154"/>
-      <c r="AC50" s="155"/>
+      <c r="Q50" s="109" t="s">
+        <v>239</v>
+      </c>
+      <c r="R50" s="153" t="s">
+        <v>88</v>
+      </c>
+      <c r="S50" s="157" t="n">
+        <v>50000.0</v>
+      </c>
+      <c r="T50" s="157" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="U50" s="152" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="V50" s="152" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="W50" s="153" t="n">
+        <v>0.03030303050763905</v>
+      </c>
+      <c r="X50" s="152" t="n">
+        <v>6.06060610152781E-4</v>
+      </c>
+      <c r="Y50" s="152" t="n">
+        <v>4.3290042877197263E-4</v>
+      </c>
+      <c r="Z50" s="152" t="n">
+        <v>0.03787878528237343</v>
+      </c>
+      <c r="AA50" s="152" t="n">
+        <v>7.575757335871458E-4</v>
+      </c>
+      <c r="AB50" s="154" t="n">
+        <v>5.411254824139178E-4</v>
+      </c>
+      <c r="AC50" s="278" t="s">
+        <v>233</v>
+      </c>
       <c r="AD50" s="39"/>
       <c r="AE50" s="42"/>
       <c r="AF50" s="42"/>

</xml_diff>